<commit_message>
Published state of ETDataset on 2 March 2016
</commit_message>
<xml_diff>
--- a/analyses/8_transport_analysis.xlsx
+++ b/analyses/8_transport_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="891" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="891" firstSheet="15" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -803,9 +803,6 @@
     <t>transport_car_using_compressed_natural_gas</t>
   </si>
   <si>
-    <t>transport_road_compressor_network_gas_parent_share</t>
-  </si>
-  <si>
     <t>transport_truck_using_compressed_natural_gas</t>
   </si>
   <si>
@@ -1214,9 +1211,6 @@
     <t>transport_final_demand_for_road_lng</t>
   </si>
   <si>
-    <t>transport_final_demand_for_road_network_gas</t>
-  </si>
-  <si>
     <t>Co-fuelling shares</t>
   </si>
   <si>
@@ -1363,9 +1357,6 @@
     <t>transport_shipping_bio_lng_ship_type</t>
   </si>
   <si>
-    <t>transport_final_demand_for_road_network_gas_parent_share</t>
-  </si>
-  <si>
     <t>transport_final_demand_for_shipping_lng</t>
   </si>
   <si>
@@ -1391,6 +1382,15 @@
   </si>
   <si>
     <t>Not taken into account</t>
+  </si>
+  <si>
+    <t>transport_final_demand_for_road_natural_gas_parent_share</t>
+  </si>
+  <si>
+    <t>transport_final_demand_for_road_compressed_network_gas</t>
+  </si>
+  <si>
+    <t>transport_road_mixer_compressed_network_gas_parent_share</t>
   </si>
 </sst>
 </file>
@@ -4730,6 +4730,7 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="9" xfId="408" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4748,19 +4749,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4775,29 +4785,19 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="2" borderId="9" xfId="408" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1728">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -8873,7 +8873,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -8935,10 +8935,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>337</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>338</v>
       </c>
       <c r="D19" s="7"/>
     </row>
@@ -8952,7 +8952,7 @@
     <row r="21" spans="2:4">
       <c r="B21" s="21"/>
       <c r="C21" s="205" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D21" s="7"/>
     </row>
@@ -8966,7 +8966,7 @@
     <row r="23" spans="2:4">
       <c r="B23" s="19"/>
       <c r="C23" s="206" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D23" s="7"/>
     </row>
@@ -9084,7 +9084,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="20">
       <c r="B2" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -9097,18 +9097,18 @@
       <c r="F4" s="136"/>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1">
-      <c r="B5" s="343" t="s">
-        <v>359</v>
-      </c>
-      <c r="C5" s="348"/>
-      <c r="D5" s="348"/>
-      <c r="E5" s="344"/>
+      <c r="B5" s="344" t="s">
+        <v>358</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="345"/>
       <c r="F5" s="111"/>
     </row>
     <row r="6" spans="2:6" ht="16" thickBot="1"/>
     <row r="7" spans="2:6">
       <c r="B7" s="28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="163"/>
@@ -9124,19 +9124,19 @@
     </row>
     <row r="9" spans="2:6" ht="30">
       <c r="B9" s="221" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C9" s="222" t="s">
+        <v>299</v>
+      </c>
+      <c r="D9" s="222" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="158" t="s">
         <v>300</v>
       </c>
-      <c r="D9" s="222" t="s">
-        <v>315</v>
-      </c>
-      <c r="E9" s="158" t="s">
+      <c r="F9" s="113" t="s">
         <v>301</v>
-      </c>
-      <c r="F9" s="113" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -9154,7 +9154,7 @@
         <v>108</v>
       </c>
       <c r="D11" s="143" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E11" s="218">
         <f>Dashboard!E30</f>
@@ -9169,7 +9169,7 @@
       <c r="B12" s="165"/>
       <c r="C12" s="214"/>
       <c r="D12" s="143" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E12" s="218">
         <f>Dashboard!E31</f>
@@ -9190,10 +9190,10 @@
     <row r="14" spans="2:6">
       <c r="B14" s="165"/>
       <c r="C14" s="214" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D14" s="143" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E14" s="218">
         <f>Dashboard!E24</f>
@@ -9208,7 +9208,7 @@
       <c r="B15" s="165"/>
       <c r="C15" s="214"/>
       <c r="D15" s="143" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E15" s="218">
         <f>Dashboard!E25</f>
@@ -9229,10 +9229,10 @@
     <row r="17" spans="2:6">
       <c r="B17" s="165"/>
       <c r="C17" s="214" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D17" s="143" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E17" s="218">
         <f>Dashboard!E27</f>
@@ -9247,7 +9247,7 @@
       <c r="B18" s="165"/>
       <c r="C18" s="214"/>
       <c r="D18" s="143" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E18" s="218">
         <f>Dashboard!E28</f>
@@ -9268,10 +9268,10 @@
     <row r="20" spans="2:6">
       <c r="B20" s="165"/>
       <c r="C20" s="214" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D20" s="143" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E20" s="218">
         <f>Dashboard!E36</f>
@@ -9286,7 +9286,7 @@
       <c r="B21" s="165"/>
       <c r="C21" s="214"/>
       <c r="D21" s="143" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E21" s="218">
         <f>Dashboard!E37</f>
@@ -9366,7 +9366,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="20">
       <c r="B2" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -9390,13 +9390,13 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="343" t="s">
-        <v>419</v>
-      </c>
-      <c r="C5" s="348"/>
-      <c r="D5" s="348"/>
-      <c r="E5" s="348"/>
-      <c r="F5" s="344"/>
+      <c r="B5" s="344" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="349"/>
+      <c r="F5" s="345"/>
     </row>
     <row r="6" spans="2:6" ht="16" customHeight="1" thickBot="1">
       <c r="B6" s="1"/>
@@ -9407,7 +9407,7 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="28" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C7" s="286"/>
       <c r="D7" s="333"/>
@@ -9421,21 +9421,21 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C9" s="160" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D9" s="332" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E9" s="162" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="211" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="334"/>
@@ -9444,7 +9444,7 @@
     <row r="11" spans="2:6">
       <c r="B11" s="165"/>
       <c r="C11" s="143" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D11" s="335">
         <f>Dashboard!E33</f>
@@ -9458,7 +9458,7 @@
     <row r="12" spans="2:6">
       <c r="B12" s="165"/>
       <c r="C12" s="143" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D12" s="337">
         <f>Dashboard!E34</f>
@@ -9472,7 +9472,7 @@
     <row r="13" spans="2:6">
       <c r="B13" s="165"/>
       <c r="C13" s="338" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D13" s="339">
         <f>SUM(D11:D12)</f>
@@ -9485,7 +9485,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="211" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="49"/>
@@ -9494,7 +9494,7 @@
     <row r="15" spans="2:6">
       <c r="B15" s="165"/>
       <c r="C15" s="143" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D15" s="335">
         <f>Dashboard!E40</f>
@@ -9508,7 +9508,7 @@
     <row r="16" spans="2:6">
       <c r="B16" s="165"/>
       <c r="C16" s="143" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D16" s="337">
         <f>Dashboard!E41</f>
@@ -9522,7 +9522,7 @@
     <row r="17" spans="2:6" ht="16" thickBot="1">
       <c r="B17" s="165"/>
       <c r="C17" s="325" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D17" s="336">
         <f>SUM(D15:D16)</f>
@@ -9541,7 +9541,7 @@
     </row>
     <row r="20" spans="2:6" ht="20">
       <c r="B20" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -9556,13 +9556,13 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="343" t="s">
-        <v>410</v>
-      </c>
-      <c r="C23" s="348"/>
-      <c r="D23" s="348"/>
-      <c r="E23" s="348"/>
-      <c r="F23" s="344"/>
+      <c r="B23" s="344" t="s">
+        <v>408</v>
+      </c>
+      <c r="C23" s="349"/>
+      <c r="D23" s="349"/>
+      <c r="E23" s="349"/>
+      <c r="F23" s="345"/>
     </row>
     <row r="24" spans="2:6" ht="15" customHeight="1" thickBot="1">
       <c r="B24" s="1"/>
@@ -9573,7 +9573,7 @@
     </row>
     <row r="25" spans="2:6" ht="15" customHeight="1">
       <c r="B25" s="28" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C25" s="321"/>
       <c r="D25" s="161"/>
@@ -9589,24 +9589,24 @@
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="36" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C27" s="160" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D27" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="E27" s="119" t="s">
+        <v>397</v>
+      </c>
+      <c r="F27" s="162" t="s">
         <v>395</v>
-      </c>
-      <c r="E27" s="119" t="s">
-        <v>399</v>
-      </c>
-      <c r="F27" s="162" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="211" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="120"/>
@@ -9616,7 +9616,7 @@
     <row r="29" spans="2:6">
       <c r="B29" s="165"/>
       <c r="C29" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D29" s="138">
         <f>'Fuel Aggregation'!I15*Dashboard!E46</f>
@@ -9634,7 +9634,7 @@
     <row r="30" spans="2:6">
       <c r="B30" s="165"/>
       <c r="C30" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D30" s="138">
         <f>'Fuel Aggregation'!K15*Dashboard!E50</f>
@@ -9652,7 +9652,7 @@
     <row r="31" spans="2:6" ht="16" thickBot="1">
       <c r="B31" s="165"/>
       <c r="C31" s="325" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D31" s="326">
         <f>SUM(D29:D30)</f>
@@ -9676,7 +9676,7 @@
     </row>
     <row r="33" spans="2:6" ht="16" customHeight="1">
       <c r="B33" s="211" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C33" s="125"/>
       <c r="D33" s="140"/>
@@ -9686,7 +9686,7 @@
     <row r="34" spans="2:6">
       <c r="B34" s="165"/>
       <c r="C34" s="323" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D34" s="138">
         <f>'Fuel Aggregation'!I15*Dashboard!E47</f>
@@ -9704,7 +9704,7 @@
     <row r="35" spans="2:6">
       <c r="B35" s="165"/>
       <c r="C35" s="323" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D35" s="138">
         <f>'Fuel Aggregation'!I15*Dashboard!E51</f>
@@ -9722,7 +9722,7 @@
     <row r="36" spans="2:6">
       <c r="B36" s="165"/>
       <c r="C36" s="323" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D36" s="138">
         <f>'Fuel Aggregation'!G15</f>
@@ -9740,7 +9740,7 @@
     <row r="37" spans="2:6">
       <c r="B37" s="165"/>
       <c r="C37" s="250" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D37" s="140">
         <f>'Fuel Aggregation'!L15</f>
@@ -9758,7 +9758,7 @@
     <row r="38" spans="2:6">
       <c r="B38" s="165"/>
       <c r="C38" s="250" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D38" s="140">
         <f>'Fuel Aggregation'!H15</f>
@@ -9776,7 +9776,7 @@
     <row r="39" spans="2:6" ht="16" thickBot="1">
       <c r="B39" s="165"/>
       <c r="C39" s="325" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D39" s="326">
         <f>SUM(D34:D38)</f>
@@ -9800,7 +9800,7 @@
     </row>
     <row r="41" spans="2:6">
       <c r="B41" s="211" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="140"/>
@@ -9810,7 +9810,7 @@
     <row r="42" spans="2:6">
       <c r="B42" s="165"/>
       <c r="C42" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D42" s="138">
         <f>'Fuel Aggregation'!I12*Dashboard!E33</f>
@@ -9828,7 +9828,7 @@
     <row r="43" spans="2:6">
       <c r="B43" s="165"/>
       <c r="C43" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D43" s="138">
         <f>'Fuel Aggregation'!K12</f>
@@ -9846,7 +9846,7 @@
     <row r="44" spans="2:6" ht="16" thickBot="1">
       <c r="B44" s="165"/>
       <c r="C44" s="325" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D44" s="326">
         <f>SUM(D42:D43)</f>
@@ -9921,30 +9921,30 @@
   <sheetData>
     <row r="2" spans="2:28" ht="20">
       <c r="B2" s="56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="2:28">
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:28">
-      <c r="B4" s="362" t="s">
+      <c r="B4" s="364" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="363"/>
-      <c r="D4" s="364"/>
+      <c r="C4" s="365"/>
+      <c r="D4" s="366"/>
     </row>
     <row r="5" spans="2:28" ht="30" customHeight="1">
-      <c r="B5" s="365" t="s">
-        <v>376</v>
-      </c>
-      <c r="C5" s="366"/>
-      <c r="D5" s="367"/>
+      <c r="B5" s="367" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="368"/>
+      <c r="D5" s="369"/>
     </row>
     <row r="6" spans="2:28" ht="16" thickBot="1"/>
     <row r="7" spans="2:28">
       <c r="B7" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C7" s="273"/>
       <c r="D7" s="273"/>
@@ -9958,20 +9958,20 @@
       <c r="L7" s="273"/>
       <c r="M7" s="273"/>
       <c r="N7" s="273"/>
-      <c r="O7" s="368"/>
-      <c r="P7" s="369"/>
-      <c r="Q7" s="369"/>
-      <c r="R7" s="369"/>
-      <c r="S7" s="369"/>
-      <c r="T7" s="369"/>
+      <c r="O7" s="370"/>
+      <c r="P7" s="371"/>
+      <c r="Q7" s="371"/>
+      <c r="R7" s="371"/>
+      <c r="S7" s="371"/>
+      <c r="T7" s="371"/>
       <c r="U7" s="247"/>
       <c r="V7" s="254"/>
       <c r="W7" s="247"/>
       <c r="X7" s="247"/>
-      <c r="Y7" s="372"/>
-      <c r="Z7" s="372"/>
-      <c r="AA7" s="372"/>
-      <c r="AB7" s="373"/>
+      <c r="Y7" s="350"/>
+      <c r="Z7" s="350"/>
+      <c r="AA7" s="350"/>
+      <c r="AB7" s="351"/>
     </row>
     <row r="8" spans="2:28">
       <c r="B8" s="36"/>
@@ -9987,24 +9987,24 @@
       <c r="L8" s="250"/>
       <c r="M8" s="250"/>
       <c r="N8" s="250"/>
-      <c r="O8" s="355"/>
-      <c r="P8" s="353"/>
-      <c r="Q8" s="353"/>
-      <c r="R8" s="353"/>
-      <c r="S8" s="353"/>
-      <c r="T8" s="353"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="356"/>
+      <c r="Q8" s="356"/>
+      <c r="R8" s="356"/>
+      <c r="S8" s="356"/>
+      <c r="T8" s="356"/>
       <c r="U8" s="245"/>
       <c r="V8" s="255"/>
       <c r="W8" s="245"/>
       <c r="X8" s="245"/>
-      <c r="Y8" s="374"/>
-      <c r="Z8" s="374"/>
-      <c r="AA8" s="374"/>
-      <c r="AB8" s="375"/>
+      <c r="Y8" s="352"/>
+      <c r="Z8" s="352"/>
+      <c r="AA8" s="352"/>
+      <c r="AB8" s="353"/>
     </row>
     <row r="9" spans="2:28" ht="45">
       <c r="B9" s="112" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C9" s="276" t="s">
         <v>200</v>
@@ -10040,28 +10040,28 @@
         <v>108</v>
       </c>
       <c r="N9" s="276" t="s">
-        <v>254</v>
-      </c>
-      <c r="O9" s="370" t="s">
-        <v>312</v>
-      </c>
-      <c r="P9" s="371"/>
-      <c r="Q9" s="371"/>
-      <c r="R9" s="371"/>
-      <c r="S9" s="371"/>
-      <c r="T9" s="371"/>
+        <v>253</v>
+      </c>
+      <c r="O9" s="373" t="s">
+        <v>311</v>
+      </c>
+      <c r="P9" s="374"/>
+      <c r="Q9" s="374"/>
+      <c r="R9" s="374"/>
+      <c r="S9" s="374"/>
+      <c r="T9" s="374"/>
       <c r="U9" s="253"/>
       <c r="V9" s="256" t="s">
         <v>89</v>
       </c>
       <c r="W9" s="58"/>
       <c r="X9" s="58"/>
-      <c r="Y9" s="351" t="s">
-        <v>312</v>
-      </c>
-      <c r="Z9" s="351"/>
-      <c r="AA9" s="351"/>
-      <c r="AB9" s="352"/>
+      <c r="Y9" s="354" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z9" s="354"/>
+      <c r="AA9" s="354"/>
+      <c r="AB9" s="355"/>
     </row>
     <row r="10" spans="2:28">
       <c r="B10" s="241"/>
@@ -10077,24 +10077,24 @@
       <c r="L10" s="242"/>
       <c r="M10" s="242"/>
       <c r="N10" s="243"/>
-      <c r="O10" s="376"/>
-      <c r="P10" s="377"/>
-      <c r="Q10" s="377"/>
-      <c r="R10" s="377"/>
-      <c r="S10" s="377"/>
-      <c r="T10" s="377"/>
-      <c r="U10" s="377"/>
+      <c r="O10" s="360"/>
+      <c r="P10" s="361"/>
+      <c r="Q10" s="361"/>
+      <c r="R10" s="361"/>
+      <c r="S10" s="361"/>
+      <c r="T10" s="361"/>
+      <c r="U10" s="361"/>
       <c r="V10" s="259"/>
       <c r="W10" s="245"/>
       <c r="X10" s="245"/>
-      <c r="Y10" s="353"/>
-      <c r="Z10" s="353"/>
-      <c r="AA10" s="353"/>
-      <c r="AB10" s="354"/>
+      <c r="Y10" s="356"/>
+      <c r="Z10" s="356"/>
+      <c r="AA10" s="356"/>
+      <c r="AB10" s="357"/>
     </row>
     <row r="11" spans="2:28">
       <c r="B11" s="115" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C11" s="235">
         <f>'Corrected energy balance step 2'!C75:S75</f>
@@ -10141,22 +10141,22 @@
         <v>0</v>
       </c>
       <c r="N11" s="234" t="s">
-        <v>288</v>
-      </c>
-      <c r="O11" s="378"/>
-      <c r="P11" s="379"/>
-      <c r="Q11" s="379"/>
-      <c r="R11" s="379"/>
-      <c r="S11" s="379"/>
-      <c r="T11" s="379"/>
-      <c r="U11" s="379"/>
+        <v>287</v>
+      </c>
+      <c r="O11" s="362"/>
+      <c r="P11" s="363"/>
+      <c r="Q11" s="363"/>
+      <c r="R11" s="363"/>
+      <c r="S11" s="363"/>
+      <c r="T11" s="363"/>
+      <c r="U11" s="363"/>
       <c r="V11" s="258"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="353"/>
-      <c r="Z11" s="353"/>
-      <c r="AA11" s="353"/>
-      <c r="AB11" s="354"/>
+      <c r="Y11" s="356"/>
+      <c r="Z11" s="356"/>
+      <c r="AA11" s="356"/>
+      <c r="AB11" s="357"/>
     </row>
     <row r="12" spans="2:28">
       <c r="B12" s="115" t="s">
@@ -10207,22 +10207,22 @@
         <v>0</v>
       </c>
       <c r="N12" s="234" t="s">
-        <v>288</v>
-      </c>
-      <c r="O12" s="360"/>
-      <c r="P12" s="361"/>
-      <c r="Q12" s="361"/>
-      <c r="R12" s="361"/>
-      <c r="S12" s="361"/>
-      <c r="T12" s="361"/>
-      <c r="U12" s="361"/>
+        <v>287</v>
+      </c>
+      <c r="O12" s="358"/>
+      <c r="P12" s="359"/>
+      <c r="Q12" s="359"/>
+      <c r="R12" s="359"/>
+      <c r="S12" s="359"/>
+      <c r="T12" s="359"/>
+      <c r="U12" s="359"/>
       <c r="V12" s="258"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="353"/>
-      <c r="Z12" s="353"/>
-      <c r="AA12" s="353"/>
-      <c r="AB12" s="354"/>
+      <c r="Y12" s="356"/>
+      <c r="Z12" s="356"/>
+      <c r="AA12" s="356"/>
+      <c r="AB12" s="357"/>
     </row>
     <row r="13" spans="2:28">
       <c r="B13" s="115" t="s">
@@ -10273,83 +10273,83 @@
         <v>0</v>
       </c>
       <c r="N13" s="234" t="s">
-        <v>288</v>
-      </c>
-      <c r="O13" s="360"/>
-      <c r="P13" s="361"/>
-      <c r="Q13" s="361"/>
-      <c r="R13" s="361"/>
-      <c r="S13" s="361"/>
-      <c r="T13" s="361"/>
-      <c r="U13" s="361"/>
+        <v>287</v>
+      </c>
+      <c r="O13" s="358"/>
+      <c r="P13" s="359"/>
+      <c r="Q13" s="359"/>
+      <c r="R13" s="359"/>
+      <c r="S13" s="359"/>
+      <c r="T13" s="359"/>
+      <c r="U13" s="359"/>
       <c r="V13" s="258"/>
       <c r="W13" s="245"/>
       <c r="X13" s="245"/>
-      <c r="Y13" s="353"/>
-      <c r="Z13" s="353"/>
-      <c r="AA13" s="353"/>
-      <c r="AB13" s="354"/>
+      <c r="Y13" s="356"/>
+      <c r="Z13" s="356"/>
+      <c r="AA13" s="356"/>
+      <c r="AB13" s="357"/>
     </row>
     <row r="14" spans="2:28">
       <c r="B14" s="115" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M14" s="234" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N14" s="270" t="s">
-        <v>288</v>
-      </c>
-      <c r="O14" s="360" t="s">
-        <v>378</v>
-      </c>
-      <c r="P14" s="361"/>
-      <c r="Q14" s="361"/>
-      <c r="R14" s="361"/>
-      <c r="S14" s="361"/>
-      <c r="T14" s="361"/>
-      <c r="U14" s="361"/>
+        <v>287</v>
+      </c>
+      <c r="O14" s="358" t="s">
+        <v>377</v>
+      </c>
+      <c r="P14" s="359"/>
+      <c r="Q14" s="359"/>
+      <c r="R14" s="359"/>
+      <c r="S14" s="359"/>
+      <c r="T14" s="359"/>
+      <c r="U14" s="359"/>
       <c r="V14" s="258"/>
       <c r="W14" s="116"/>
       <c r="X14" s="116"/>
-      <c r="Y14" s="353"/>
-      <c r="Z14" s="353"/>
-      <c r="AA14" s="353"/>
-      <c r="AB14" s="354"/>
+      <c r="Y14" s="356"/>
+      <c r="Z14" s="356"/>
+      <c r="AA14" s="356"/>
+      <c r="AB14" s="357"/>
     </row>
     <row r="15" spans="2:28">
       <c r="B15" s="115" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C15" s="235">
         <f>'Corrected energy balance step 2'!C79:S79</f>
@@ -10396,75 +10396,75 @@
         <v>0</v>
       </c>
       <c r="N15" s="234" t="s">
-        <v>288</v>
-      </c>
-      <c r="O15" s="360"/>
-      <c r="P15" s="361"/>
-      <c r="Q15" s="361"/>
-      <c r="R15" s="361"/>
-      <c r="S15" s="361"/>
-      <c r="T15" s="361"/>
-      <c r="U15" s="361"/>
+        <v>287</v>
+      </c>
+      <c r="O15" s="358"/>
+      <c r="P15" s="359"/>
+      <c r="Q15" s="359"/>
+      <c r="R15" s="359"/>
+      <c r="S15" s="359"/>
+      <c r="T15" s="359"/>
+      <c r="U15" s="359"/>
       <c r="V15" s="261"/>
       <c r="W15" s="58"/>
       <c r="X15" s="58"/>
-      <c r="Y15" s="351"/>
-      <c r="Z15" s="351"/>
-      <c r="AA15" s="351"/>
-      <c r="AB15" s="352"/>
+      <c r="Y15" s="354"/>
+      <c r="Z15" s="354"/>
+      <c r="AA15" s="354"/>
+      <c r="AB15" s="355"/>
     </row>
     <row r="16" spans="2:28">
       <c r="B16" s="114" t="s">
         <v>165</v>
       </c>
       <c r="C16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G16" s="236">
         <f>'Corrected energy balance step 2'!AI80</f>
         <v>0</v>
       </c>
       <c r="H16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M16" s="236" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N16" s="236" t="s">
-        <v>288</v>
-      </c>
-      <c r="O16" s="360" t="s">
-        <v>379</v>
-      </c>
-      <c r="P16" s="361"/>
-      <c r="Q16" s="361"/>
-      <c r="R16" s="361"/>
-      <c r="S16" s="361"/>
-      <c r="T16" s="361"/>
-      <c r="U16" s="361"/>
+        <v>287</v>
+      </c>
+      <c r="O16" s="358" t="s">
+        <v>378</v>
+      </c>
+      <c r="P16" s="359"/>
+      <c r="Q16" s="359"/>
+      <c r="R16" s="359"/>
+      <c r="S16" s="359"/>
+      <c r="T16" s="359"/>
+      <c r="U16" s="359"/>
       <c r="V16" s="257" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="W16" s="245"/>
       <c r="X16" s="245"/>
@@ -10487,16 +10487,16 @@
       <c r="L17" s="230"/>
       <c r="M17" s="230"/>
       <c r="N17" s="230"/>
-      <c r="O17" s="355"/>
-      <c r="P17" s="353"/>
-      <c r="Q17" s="353"/>
-      <c r="R17" s="353"/>
-      <c r="S17" s="353"/>
-      <c r="T17" s="353"/>
-      <c r="U17" s="353"/>
+      <c r="O17" s="372"/>
+      <c r="P17" s="356"/>
+      <c r="Q17" s="356"/>
+      <c r="R17" s="356"/>
+      <c r="S17" s="356"/>
+      <c r="T17" s="356"/>
+      <c r="U17" s="356"/>
       <c r="V17" s="258"/>
       <c r="W17" s="262" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="X17" s="116"/>
       <c r="Y17" s="250"/>
@@ -10509,51 +10509,51 @@
         <v>174</v>
       </c>
       <c r="C18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M18" s="237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N18" s="237">
         <f>'Corrected energy balance step 2'!BN90</f>
         <v>0</v>
       </c>
-      <c r="O18" s="358" t="s">
-        <v>313</v>
-      </c>
-      <c r="P18" s="359"/>
-      <c r="Q18" s="359"/>
-      <c r="R18" s="359"/>
-      <c r="S18" s="359"/>
-      <c r="T18" s="359"/>
-      <c r="U18" s="359"/>
+      <c r="O18" s="379" t="s">
+        <v>312</v>
+      </c>
+      <c r="P18" s="380"/>
+      <c r="Q18" s="380"/>
+      <c r="R18" s="380"/>
+      <c r="S18" s="380"/>
+      <c r="T18" s="380"/>
+      <c r="U18" s="380"/>
       <c r="V18" s="258"/>
       <c r="AB18" s="246"/>
     </row>
@@ -10571,16 +10571,16 @@
       <c r="L19" s="232"/>
       <c r="M19" s="232"/>
       <c r="N19" s="232"/>
-      <c r="O19" s="356"/>
-      <c r="P19" s="357"/>
-      <c r="Q19" s="357"/>
-      <c r="R19" s="357"/>
-      <c r="S19" s="357"/>
-      <c r="T19" s="357"/>
-      <c r="U19" s="357"/>
+      <c r="O19" s="377"/>
+      <c r="P19" s="378"/>
+      <c r="Q19" s="378"/>
+      <c r="R19" s="378"/>
+      <c r="S19" s="378"/>
+      <c r="T19" s="378"/>
+      <c r="U19" s="378"/>
       <c r="V19" s="258"/>
       <c r="W19" s="209" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="X19" s="227">
         <f>ROUND(SUM($C$21:$N$22),-1)</f>
@@ -10605,16 +10605,16 @@
       <c r="L20" s="274"/>
       <c r="M20" s="274"/>
       <c r="N20" s="274"/>
-      <c r="O20" s="355"/>
-      <c r="P20" s="353"/>
-      <c r="Q20" s="353"/>
-      <c r="R20" s="353"/>
-      <c r="S20" s="353"/>
-      <c r="T20" s="353"/>
-      <c r="U20" s="353"/>
+      <c r="O20" s="372"/>
+      <c r="P20" s="356"/>
+      <c r="Q20" s="356"/>
+      <c r="R20" s="356"/>
+      <c r="S20" s="356"/>
+      <c r="T20" s="356"/>
+      <c r="U20" s="356"/>
       <c r="V20" s="258"/>
       <c r="W20" s="209" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="X20" s="227">
         <f>ROUND(SUM('Corrected energy balance step 2'!BN75+'Corrected energy balance step 2'!BN76+'Corrected energy balance step 2'!BN77+'Corrected energy balance step 2'!BN79+'Corrected energy balance step 2'!BN90),-1)</f>
@@ -10627,7 +10627,7 @@
     </row>
     <row r="21" spans="2:41">
       <c r="B21" s="229" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C21" s="210">
         <f t="shared" ref="C21:H21" si="0">SUM(C11:C16)</f>
@@ -10674,15 +10674,15 @@
         <v>0</v>
       </c>
       <c r="N21" s="238" t="s">
-        <v>288</v>
-      </c>
-      <c r="O21" s="356"/>
-      <c r="P21" s="357"/>
-      <c r="Q21" s="357"/>
-      <c r="R21" s="357"/>
-      <c r="S21" s="357"/>
-      <c r="T21" s="357"/>
-      <c r="U21" s="357"/>
+        <v>287</v>
+      </c>
+      <c r="O21" s="377"/>
+      <c r="P21" s="378"/>
+      <c r="Q21" s="378"/>
+      <c r="R21" s="378"/>
+      <c r="S21" s="378"/>
+      <c r="T21" s="378"/>
+      <c r="U21" s="378"/>
       <c r="V21" s="258"/>
       <c r="W21" s="245"/>
       <c r="X21" s="245"/>
@@ -10693,52 +10693,52 @@
     </row>
     <row r="22" spans="2:41">
       <c r="B22" s="114" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M22" s="239" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N22" s="240">
         <f>N18</f>
         <v>0</v>
       </c>
-      <c r="O22" s="356"/>
-      <c r="P22" s="357"/>
-      <c r="Q22" s="357"/>
-      <c r="R22" s="357"/>
-      <c r="S22" s="357"/>
-      <c r="T22" s="357"/>
-      <c r="U22" s="357"/>
+      <c r="O22" s="377"/>
+      <c r="P22" s="378"/>
+      <c r="Q22" s="378"/>
+      <c r="R22" s="378"/>
+      <c r="S22" s="378"/>
+      <c r="T22" s="378"/>
+      <c r="U22" s="378"/>
       <c r="V22" s="258"/>
       <c r="W22" s="245"/>
       <c r="X22" s="245"/>
@@ -10774,13 +10774,13 @@
       <c r="L23" s="277"/>
       <c r="M23" s="277"/>
       <c r="N23" s="277"/>
-      <c r="O23" s="349"/>
-      <c r="P23" s="350"/>
-      <c r="Q23" s="350"/>
-      <c r="R23" s="350"/>
-      <c r="S23" s="350"/>
-      <c r="T23" s="350"/>
-      <c r="U23" s="350"/>
+      <c r="O23" s="375"/>
+      <c r="P23" s="376"/>
+      <c r="Q23" s="376"/>
+      <c r="R23" s="376"/>
+      <c r="S23" s="376"/>
+      <c r="T23" s="376"/>
+      <c r="U23" s="376"/>
       <c r="V23" s="260"/>
       <c r="W23" s="248"/>
       <c r="X23" s="248"/>
@@ -10806,14 +10806,31 @@
       <c r="V24" s="245"/>
       <c r="W24" s="116"/>
       <c r="X24" s="116"/>
-      <c r="Y24" s="353"/>
-      <c r="Z24" s="353"/>
-      <c r="AA24" s="353"/>
-      <c r="AB24" s="353"/>
+      <c r="Y24" s="356"/>
+      <c r="Z24" s="356"/>
+      <c r="AA24" s="356"/>
+      <c r="AB24" s="356"/>
       <c r="AC24" s="245"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="O23:U23"/>
+    <mergeCell ref="Y15:AB15"/>
+    <mergeCell ref="Y24:AB24"/>
+    <mergeCell ref="Y13:AB13"/>
+    <mergeCell ref="O20:U20"/>
+    <mergeCell ref="O21:U21"/>
+    <mergeCell ref="O22:U22"/>
+    <mergeCell ref="O18:U18"/>
+    <mergeCell ref="O19:U19"/>
+    <mergeCell ref="O15:U15"/>
+    <mergeCell ref="O16:U16"/>
+    <mergeCell ref="O17:U17"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="O8:T8"/>
+    <mergeCell ref="O9:T9"/>
     <mergeCell ref="Y7:AB7"/>
     <mergeCell ref="Y8:AB8"/>
     <mergeCell ref="Y9:AB9"/>
@@ -10826,23 +10843,6 @@
     <mergeCell ref="O10:U10"/>
     <mergeCell ref="O11:U11"/>
     <mergeCell ref="O12:U12"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="O8:T8"/>
-    <mergeCell ref="O9:T9"/>
-    <mergeCell ref="O23:U23"/>
-    <mergeCell ref="Y15:AB15"/>
-    <mergeCell ref="Y24:AB24"/>
-    <mergeCell ref="Y13:AB13"/>
-    <mergeCell ref="O20:U20"/>
-    <mergeCell ref="O21:U21"/>
-    <mergeCell ref="O22:U22"/>
-    <mergeCell ref="O18:U18"/>
-    <mergeCell ref="O19:U19"/>
-    <mergeCell ref="O15:U15"/>
-    <mergeCell ref="O16:U16"/>
-    <mergeCell ref="O17:U17"/>
   </mergeCells>
   <conditionalFormatting sqref="X19:X20">
     <cfRule type="duplicateValues" dxfId="2" priority="5"/>
@@ -10885,10 +10885,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -10942,10 +10942,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -11014,10 +11014,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11071,10 +11071,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11137,10 +11137,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11197,10 +11197,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11254,10 +11254,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11271,7 +11271,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" s="159">
         <f>'Technology Shares'!F15</f>
@@ -11349,7 +11349,7 @@
         <v>41481</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D7" s="27"/>
     </row>
@@ -11358,7 +11358,7 @@
         <v>41488</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D8" s="27">
         <v>2</v>
@@ -11369,7 +11369,7 @@
         <v>41498</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D9" s="18">
         <v>2.0099999999999998</v>
@@ -11380,7 +11380,7 @@
         <v>41499</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D10" s="18">
         <v>2.02</v>
@@ -11391,7 +11391,7 @@
         <v>41499</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D11" s="18">
         <v>2.0299999999999998</v>
@@ -11402,7 +11402,7 @@
         <v>41500</v>
       </c>
       <c r="C12" s="244" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D12" s="18">
         <v>2.04</v>
@@ -11413,7 +11413,7 @@
         <v>41507</v>
       </c>
       <c r="C13" s="268" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D13" s="18">
         <v>2.0499999999999998</v>
@@ -11424,7 +11424,7 @@
         <v>41509</v>
       </c>
       <c r="C14" s="269" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D14" s="18">
         <v>2.06</v>
@@ -11435,7 +11435,7 @@
         <v>41536</v>
       </c>
       <c r="C15" s="275" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D15" s="18">
         <v>2.0699999999999998</v>
@@ -11446,7 +11446,7 @@
         <v>41556</v>
       </c>
       <c r="C16" s="279" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D16" s="18">
         <v>2.08</v>
@@ -11457,7 +11457,7 @@
         <v>41562</v>
       </c>
       <c r="C17" s="268" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D17" s="18">
         <v>2.09</v>
@@ -11468,7 +11468,7 @@
         <v>42299</v>
       </c>
       <c r="C18" s="283" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D18" s="18">
         <v>2.1</v>
@@ -11562,10 +11562,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11605,7 +11605,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11616,15 +11616,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -11638,7 +11638,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="159">
         <f>'Technology Shares'!F21</f>
@@ -11664,7 +11664,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11675,20 +11675,20 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B3" s="159">
         <f>'Fuelling shares'!D15</f>
@@ -11697,7 +11697,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>387</v>
+        <v>444</v>
       </c>
       <c r="B4" s="159">
         <f>'Fuelling shares'!D16</f>
@@ -11722,8 +11722,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11734,20 +11734,20 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3">
         <f>'Fuelling shares'!D11</f>
@@ -11756,7 +11756,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>387</v>
+        <v>444</v>
       </c>
       <c r="B4">
         <f>'Fuelling shares'!D12</f>
@@ -11791,20 +11791,20 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B3" s="328">
         <f>'Fuelling shares'!E42</f>
@@ -11813,7 +11813,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B4" s="328">
         <f>'Fuelling shares'!E43</f>
@@ -11852,20 +11852,20 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="341" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B3" s="328">
         <f>'Fuelling shares'!E34</f>
@@ -11874,7 +11874,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="341" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B4" s="328">
         <f xml:space="preserve"> 'Fuelling shares'!E35</f>
@@ -11901,7 +11901,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="341" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B7" s="328">
         <f xml:space="preserve"> 'Fuelling shares'!E38</f>
@@ -11936,20 +11936,20 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
         <v>272</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="341" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3" s="328">
         <f>'Fuelling shares'!E29</f>
@@ -11958,7 +11958,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="341" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B4" s="328">
         <f xml:space="preserve"> 'Fuelling shares'!E30</f>
@@ -12010,7 +12010,7 @@
     </row>
     <row r="6" spans="2:2" ht="45">
       <c r="B6" s="67" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="2:2">
@@ -12026,32 +12026,32 @@
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="86" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="86" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="86" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="86" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="86" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="86" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="2:2">
@@ -12059,7 +12059,7 @@
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="66" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -12067,7 +12067,7 @@
     </row>
     <row r="20" spans="2:2" ht="90">
       <c r="B20" s="208" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="2:2">
@@ -12173,12 +12173,12 @@
         <v>27</v>
       </c>
       <c r="C12" s="201" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28" customHeight="1">
       <c r="B13" s="202" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>87</v>
@@ -12186,18 +12186,18 @@
     </row>
     <row r="14" spans="2:3" ht="28" customHeight="1">
       <c r="B14" s="266" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C14" s="203" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="28" customHeight="1">
       <c r="B15" s="266" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C15" s="203" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="28" customHeight="1">
@@ -12205,119 +12205,119 @@
         <v>201</v>
       </c>
       <c r="C16" s="201" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="28" customHeight="1">
       <c r="B17" s="80" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C17" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="28" customHeight="1">
       <c r="B18" s="80" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C18" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="28" customHeight="1">
       <c r="B19" s="80" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C19" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="28" customHeight="1">
       <c r="B20" s="80" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C20" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="28" customHeight="1">
       <c r="B21" s="80" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C21" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="28" customHeight="1">
       <c r="B22" s="80" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C22" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="28" customHeight="1">
       <c r="B23" s="80" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C23" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="28" customHeight="1">
       <c r="B24" s="80" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C24" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="28" customHeight="1">
       <c r="B25" s="80" t="s">
+        <v>334</v>
+      </c>
+      <c r="C25" s="201" t="s">
         <v>335</v>
-      </c>
-      <c r="C25" s="201" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="28" customHeight="1">
       <c r="B26" s="80" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C26" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="25" customHeight="1">
       <c r="B27" s="80" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C27" s="201" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="25" customHeight="1">
       <c r="B28" s="80" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C28" s="201" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="26" customHeight="1">
       <c r="B29" s="80" t="s">
+        <v>414</v>
+      </c>
+      <c r="C29" s="201" t="s">
         <v>416</v>
-      </c>
-      <c r="C29" s="201" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="25" customHeight="1">
       <c r="B30" s="80" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C30" s="201" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -12351,7 +12351,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="20" customHeight="1">
       <c r="B2" s="72" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
@@ -12741,10 +12741,10 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:4" ht="79" customHeight="1">
-      <c r="B5" s="343" t="s">
+      <c r="B5" s="344" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="344"/>
+      <c r="C5" s="345"/>
     </row>
     <row r="6" spans="2:4" ht="16" thickBot="1"/>
     <row r="7" spans="2:4">
@@ -12780,14 +12780,14 @@
     <row r="11" spans="2:4" ht="15" customHeight="1">
       <c r="B11" s="39"/>
       <c r="C11" s="60" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D11" s="40"/>
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1">
       <c r="B12" s="39"/>
       <c r="C12" s="57" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D12" s="88"/>
     </row>
@@ -12801,21 +12801,21 @@
     <row r="14" spans="2:4" ht="15" customHeight="1">
       <c r="B14" s="39"/>
       <c r="C14" s="127" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D14" s="88"/>
     </row>
     <row r="15" spans="2:4" ht="15" customHeight="1">
       <c r="B15" s="39"/>
       <c r="C15" s="127" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="88"/>
     </row>
     <row r="16" spans="2:4" ht="15" customHeight="1">
       <c r="B16" s="39"/>
       <c r="C16" s="127" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D16" s="88"/>
     </row>
@@ -12829,28 +12829,28 @@
     <row r="18" spans="2:4" ht="15" customHeight="1">
       <c r="B18" s="39"/>
       <c r="C18" s="57" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D18" s="88"/>
     </row>
     <row r="19" spans="2:4" ht="15" customHeight="1">
       <c r="B19" s="39"/>
       <c r="C19" s="127" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D19" s="88"/>
     </row>
     <row r="20" spans="2:4" ht="15" customHeight="1">
       <c r="B20" s="39"/>
       <c r="C20" s="127" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D20" s="88"/>
     </row>
     <row r="21" spans="2:4" ht="15" customHeight="1">
       <c r="B21" s="39"/>
       <c r="C21" s="127" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D21" s="88"/>
     </row>
@@ -12892,7 +12892,7 @@
     <row r="27" spans="2:4" ht="15" customHeight="1">
       <c r="B27" s="39"/>
       <c r="C27" s="65" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D27" s="88"/>
     </row>
@@ -12906,21 +12906,21 @@
     <row r="29" spans="2:4" ht="15" customHeight="1">
       <c r="B29" s="39"/>
       <c r="C29" s="127" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D29" s="88"/>
     </row>
     <row r="30" spans="2:4" ht="15" customHeight="1">
       <c r="B30" s="39"/>
       <c r="C30" s="127" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D30" s="88"/>
     </row>
     <row r="31" spans="2:4" ht="15" customHeight="1">
       <c r="B31" s="39"/>
       <c r="C31" s="65" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D31" s="88"/>
     </row>
@@ -12953,14 +12953,14 @@
     <row r="36" spans="2:9" ht="30" customHeight="1">
       <c r="B36" s="39"/>
       <c r="C36" s="118" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D36" s="88"/>
     </row>
     <row r="37" spans="2:9" ht="15" customHeight="1">
       <c r="B37" s="39"/>
       <c r="C37" s="233" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D37" s="88"/>
     </row>
@@ -12998,7 +12998,7 @@
     </row>
     <row r="43" spans="2:9">
       <c r="B43" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="37"/>
@@ -13009,7 +13009,7 @@
         <v>208</v>
       </c>
       <c r="D44" s="101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="2:9">
@@ -13032,7 +13032,7 @@
         <v>212</v>
       </c>
       <c r="D47" s="101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="2:9">
@@ -13054,7 +13054,7 @@
         <v>213</v>
       </c>
       <c r="D50" s="101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="2:9">
@@ -13326,7 +13326,7 @@
     </row>
     <row r="99" spans="2:3">
       <c r="B99" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C99" s="99" t="s">
         <v>80</v>
@@ -13386,10 +13386,10 @@
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" s="98" t="s">
         <v>254</v>
-      </c>
-      <c r="C110" s="98" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="16" thickBot="1">
@@ -13417,7 +13417,9 @@
   </sheetPr>
   <dimension ref="B1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -13456,7 +13458,7 @@
       <c r="E2" s="104"/>
       <c r="F2" s="104"/>
       <c r="I2" s="151" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J2" s="176"/>
       <c r="K2" s="13"/>
@@ -13487,12 +13489,12 @@
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="54" customHeight="1">
-      <c r="B5" s="345" t="s">
-        <v>285</v>
-      </c>
-      <c r="C5" s="346"/>
-      <c r="D5" s="346"/>
-      <c r="E5" s="347"/>
+      <c r="B5" s="346" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="347"/>
+      <c r="D5" s="347"/>
+      <c r="E5" s="348"/>
       <c r="F5" s="111"/>
       <c r="I5" s="154"/>
       <c r="J5" s="179"/>
@@ -13559,7 +13561,7 @@
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H9" s="34"/>
       <c r="I9" s="34" t="s">
@@ -13577,10 +13579,10 @@
       </c>
       <c r="N9" s="15"/>
       <c r="O9" s="171" t="s">
+        <v>317</v>
+      </c>
+      <c r="P9" s="172" t="s">
         <v>318</v>
-      </c>
-      <c r="P9" s="172" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -13610,11 +13612,11 @@
       <c r="E11" s="214"/>
       <c r="F11" s="15"/>
       <c r="G11" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H11" s="15"/>
       <c r="K11" s="49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L11" s="278" t="b">
         <f>IF(COUNTIF(P:P,0)+COUNTIF(P:P,FALSE)=0,TRUE,FALSE)</f>
@@ -13625,24 +13627,24 @@
         <v>Please address all critical checks (red) before continuing</v>
       </c>
       <c r="O11" s="153" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P11" s="166"/>
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="36"/>
       <c r="C12" s="136" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="214"/>
       <c r="F12" s="15"/>
       <c r="G12" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H12" s="15"/>
       <c r="K12" s="55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L12" s="278" t="b">
         <f>IF(COUNTBLANK(C23:C51)-COUNTBLANK(E23:E51)=0,TRUE,FALSE)</f>
@@ -13653,7 +13655,7 @@
         <v>Did you fill in all required fields in colomn E?</v>
       </c>
       <c r="O12" s="153" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P12" s="166">
         <f>IF(L12=TRUE,1,0)</f>
@@ -13678,7 +13680,7 @@
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="165" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C14" s="182"/>
       <c r="D14" s="189"/>
@@ -13696,10 +13698,10 @@
     <row r="15" spans="2:16">
       <c r="B15" s="117"/>
       <c r="C15" s="184" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D15" s="180" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E15" s="192">
         <f>'Fuel Aggregation'!X19</f>
@@ -13736,7 +13738,7 @@
         <v>161</v>
       </c>
       <c r="D17" s="180" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E17" s="196">
         <f>SUM('Fuel Aggregation'!C12:N12)</f>
@@ -13758,7 +13760,7 @@
         <v>162</v>
       </c>
       <c r="D18" s="180" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E18" s="196">
         <f>SUM('Fuel Aggregation'!C13:N13)</f>
@@ -13777,10 +13779,10 @@
     <row r="19" spans="2:16">
       <c r="B19" s="117"/>
       <c r="C19" s="185" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D19" s="180" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E19" s="196">
         <f>SUM('Fuel Aggregation'!C11:N11)</f>
@@ -13799,10 +13801,10 @@
     <row r="20" spans="2:16">
       <c r="B20" s="117"/>
       <c r="C20" s="185" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D20" s="180" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E20" s="196">
         <f>SUM('Fuel Aggregation'!C15:N15)</f>
@@ -13821,10 +13823,10 @@
     <row r="21" spans="2:16">
       <c r="B21" s="117"/>
       <c r="C21" s="185" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D21" s="180" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E21" s="196">
         <f>SUM('Fuel Aggregation'!C18:N18)</f>
@@ -13879,7 +13881,7 @@
         <v>208</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E24" s="109"/>
       <c r="F24" s="174"/>
@@ -13890,7 +13892,7 @@
       <c r="L24" s="19"/>
       <c r="M24" s="50"/>
       <c r="O24" s="153" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P24" s="166"/>
     </row>
@@ -13900,7 +13902,7 @@
         <v>209</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E25" s="110">
         <f>1-E24</f>
@@ -13937,7 +13939,7 @@
         <v>210</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E27" s="109"/>
       <c r="F27" s="174"/>
@@ -13948,7 +13950,7 @@
       <c r="L27" s="19"/>
       <c r="M27" s="50"/>
       <c r="O27" s="153" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P27" s="166"/>
     </row>
@@ -13958,7 +13960,7 @@
         <v>211</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E28" s="110">
         <f>1-E27</f>
@@ -13995,7 +13997,7 @@
         <v>212</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E30" s="109"/>
       <c r="F30" s="174"/>
@@ -14006,7 +14008,7 @@
       <c r="L30" s="19"/>
       <c r="M30" s="50"/>
       <c r="O30" s="153" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P30" s="166"/>
     </row>
@@ -14016,7 +14018,7 @@
         <v>222</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E31" s="110">
         <f>1-E30</f>
@@ -14050,27 +14052,27 @@
     <row r="33" spans="2:16" ht="16" thickBot="1">
       <c r="B33" s="31"/>
       <c r="C33" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D33" s="250" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E33" s="109"/>
       <c r="I33" s="23"/>
       <c r="K33" s="49"/>
       <c r="M33" s="50"/>
       <c r="O33" s="153" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="P33" s="166"/>
     </row>
     <row r="34" spans="2:16">
       <c r="B34" s="31"/>
       <c r="C34" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D34" s="250" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E34" s="110">
         <f>1-E33</f>
@@ -14102,7 +14104,7 @@
         <v>213</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E36" s="109"/>
       <c r="F36" s="174"/>
@@ -14113,7 +14115,7 @@
       <c r="L36" s="19"/>
       <c r="M36" s="50"/>
       <c r="O36" s="153" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P36" s="166"/>
     </row>
@@ -14123,7 +14125,7 @@
         <v>223</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E37" s="110">
         <f>1-E36</f>
@@ -14157,10 +14159,10 @@
     <row r="39" spans="2:16" ht="16" thickBot="1">
       <c r="B39" s="31"/>
       <c r="C39" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E39" s="196">
         <f>'Fuel Aggregation'!K12</f>
@@ -14179,10 +14181,10 @@
     <row r="40" spans="2:16" ht="16" thickBot="1">
       <c r="B40" s="31"/>
       <c r="C40" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E40" s="109"/>
       <c r="H40" s="250"/>
@@ -14192,17 +14194,17 @@
       <c r="L40" s="19"/>
       <c r="M40" s="50"/>
       <c r="O40" s="153" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="P40" s="166"/>
     </row>
     <row r="41" spans="2:16">
       <c r="B41" s="31"/>
       <c r="C41" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E41" s="110">
         <f>1-E40</f>
@@ -14236,7 +14238,7 @@
     </row>
     <row r="43" spans="2:16">
       <c r="B43" s="38" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C43" s="250"/>
       <c r="D43" s="52"/>
@@ -14266,10 +14268,10 @@
     <row r="45" spans="2:16" ht="16" thickBot="1">
       <c r="B45" s="31"/>
       <c r="C45" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E45" s="196">
         <f>'Fuel Aggregation'!I15</f>
@@ -14286,29 +14288,29 @@
     <row r="46" spans="2:16" ht="16" thickBot="1">
       <c r="B46" s="31"/>
       <c r="C46" s="250" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D46" s="250" t="s">
-        <v>321</v>
-      </c>
-      <c r="E46" s="380"/>
+        <v>320</v>
+      </c>
+      <c r="E46" s="343"/>
       <c r="I46" s="23"/>
       <c r="J46" s="250"/>
       <c r="K46" s="186"/>
       <c r="L46" s="19"/>
       <c r="M46" s="50"/>
       <c r="O46" s="153" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="P46" s="166"/>
     </row>
     <row r="47" spans="2:16">
       <c r="B47" s="31"/>
       <c r="C47" s="250" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D47" s="250" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E47" s="110">
         <f>1-E46</f>
@@ -14335,10 +14337,10 @@
     <row r="49" spans="2:16" ht="16" thickBot="1">
       <c r="B49" s="31"/>
       <c r="C49" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E49" s="196">
         <f>'Fuel Aggregation'!K15</f>
@@ -14355,10 +14357,10 @@
     <row r="50" spans="2:16" ht="16" thickBot="1">
       <c r="B50" s="31"/>
       <c r="C50" s="250" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D50" s="250" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E50" s="342"/>
       <c r="I50" s="23"/>
@@ -14367,17 +14369,17 @@
       <c r="L50" s="19"/>
       <c r="M50" s="50"/>
       <c r="O50" s="153" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="P50" s="166"/>
     </row>
     <row r="51" spans="2:16">
       <c r="B51" s="31"/>
       <c r="C51" s="250" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D51" s="250" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E51" s="110">
         <f>1-E50</f>
@@ -14535,7 +14537,7 @@
   <sheetData>
     <row r="2" spans="2:67" ht="20">
       <c r="B2" s="288" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="2:67" ht="15" customHeight="1">
@@ -14554,7 +14556,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1">
       <c r="B5" s="293" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C5" s="294"/>
       <c r="D5" s="295"/>
@@ -16168,7 +16170,7 @@
     </row>
     <row r="28" spans="2:67">
       <c r="B28" s="304" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C28" s="309"/>
       <c r="D28" s="309"/>
@@ -16238,7 +16240,7 @@
     </row>
     <row r="29" spans="2:67">
       <c r="B29" s="304" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C29" s="309"/>
       <c r="D29" s="309"/>
@@ -16308,7 +16310,7 @@
     </row>
     <row r="30" spans="2:67">
       <c r="B30" s="304" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C30" s="309"/>
       <c r="D30" s="309"/>
@@ -16378,7 +16380,7 @@
     </row>
     <row r="31" spans="2:67">
       <c r="B31" s="304" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C31" s="309"/>
       <c r="D31" s="309"/>
@@ -16448,7 +16450,7 @@
     </row>
     <row r="32" spans="2:67">
       <c r="B32" s="304" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C32" s="309"/>
       <c r="D32" s="309"/>
@@ -16518,7 +16520,7 @@
     </row>
     <row r="33" spans="2:67">
       <c r="B33" s="304" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C33" s="309"/>
       <c r="D33" s="309"/>
@@ -16658,7 +16660,7 @@
     </row>
     <row r="35" spans="2:67">
       <c r="B35" s="304" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C35" s="309"/>
       <c r="D35" s="309"/>
@@ -16728,7 +16730,7 @@
     </row>
     <row r="36" spans="2:67">
       <c r="B36" s="304" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C36" s="309"/>
       <c r="D36" s="309"/>
@@ -17218,7 +17220,7 @@
     </row>
     <row r="43" spans="2:67">
       <c r="B43" s="304" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C43" s="309"/>
       <c r="D43" s="309"/>
@@ -17288,7 +17290,7 @@
     </row>
     <row r="44" spans="2:67">
       <c r="B44" s="304" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C44" s="309"/>
       <c r="D44" s="309"/>
@@ -17428,7 +17430,7 @@
     </row>
     <row r="46" spans="2:67">
       <c r="B46" s="304" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C46" s="309"/>
       <c r="D46" s="309"/>
@@ -17498,7 +17500,7 @@
     </row>
     <row r="47" spans="2:67">
       <c r="B47" s="304" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C47" s="309"/>
       <c r="D47" s="309"/>
@@ -17568,7 +17570,7 @@
     </row>
     <row r="48" spans="2:67">
       <c r="B48" s="304" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C48" s="309"/>
       <c r="D48" s="309"/>
@@ -17638,7 +17640,7 @@
     </row>
     <row r="49" spans="2:67">
       <c r="B49" s="304" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C49" s="309"/>
       <c r="D49" s="309"/>
@@ -17708,7 +17710,7 @@
     </row>
     <row r="50" spans="2:67">
       <c r="B50" s="304" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C50" s="309"/>
       <c r="D50" s="309"/>
@@ -17848,7 +17850,7 @@
     </row>
     <row r="52" spans="2:67">
       <c r="B52" s="304" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C52" s="309"/>
       <c r="D52" s="309"/>
@@ -21372,7 +21374,7 @@
   </sheetPr>
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -21388,7 +21390,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="20">
       <c r="B2" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -21401,18 +21403,18 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1">
-      <c r="B5" s="343" t="s">
-        <v>360</v>
-      </c>
-      <c r="C5" s="348"/>
-      <c r="D5" s="348"/>
-      <c r="E5" s="344"/>
+      <c r="B5" s="344" t="s">
+        <v>359</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="345"/>
       <c r="F5" s="118"/>
     </row>
     <row r="6" spans="2:6" ht="16" thickBot="1"/>
     <row r="7" spans="2:6">
       <c r="B7" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="161"/>
@@ -21426,16 +21428,16 @@
     </row>
     <row r="9" spans="2:6" ht="30">
       <c r="B9" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C9" s="160" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D9" s="119" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E9" s="162" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F9" s="119"/>
     </row>
@@ -21465,7 +21467,7 @@
     <row r="12" spans="2:6">
       <c r="B12" s="165"/>
       <c r="C12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D12" s="138">
         <f>'Fuel Aggregation'!E11</f>
@@ -21523,7 +21525,7 @@
     <row r="17" spans="2:6">
       <c r="B17" s="165"/>
       <c r="C17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D17" s="138">
         <f>'Fuel Aggregation'!G15</f>
@@ -21537,14 +21539,14 @@
     <row r="18" spans="2:6">
       <c r="B18" s="165"/>
       <c r="C18" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D18" s="138">
         <f>'Fuel Aggregation'!G16</f>
         <v>0</v>
       </c>
       <c r="E18" s="122" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -21566,7 +21568,7 @@
     <row r="21" spans="2:6">
       <c r="B21" s="165"/>
       <c r="C21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D21" s="138">
         <f>'Fuel Aggregation'!J11</f>
@@ -21641,7 +21643,7 @@
     <row r="27" spans="2:6">
       <c r="B27" s="165"/>
       <c r="C27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D27" s="138">
         <f>'Fuel Aggregation'!L15</f>

</xml_diff>

<commit_message>
Published state of ETDataset on 07 december 2017
</commit_message>
<xml_diff>
--- a/analyses/8_transport_analysis.xlsx
+++ b/analyses/8_transport_analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorinevandervlies/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="891" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="891" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -33,18 +33,18 @@
     <sheet name="csv_road_gasoline_mix" sheetId="55" r:id="rId19"/>
     <sheet name="csv_road_diesel_mix" sheetId="56" r:id="rId20"/>
     <sheet name="csv_rail_diesel_mix" sheetId="72" r:id="rId21"/>
-    <sheet name="csv_rail_coal" sheetId="74" r:id="rId22"/>
-    <sheet name="csv_rail_electricity" sheetId="73" r:id="rId23"/>
-    <sheet name="csv_lng_mix" sheetId="75" r:id="rId24"/>
-    <sheet name="csv_network_gas_mix" sheetId="52" r:id="rId25"/>
-    <sheet name="csv_final_demand_road_greengas" sheetId="70" r:id="rId26"/>
-    <sheet name="csv_final_demand_natural_gas" sheetId="63" r:id="rId27"/>
-    <sheet name="csv_shipping_mixer_lng" sheetId="67" r:id="rId28"/>
-    <sheet name="csv_shipping_mixer_diesel" sheetId="69" r:id="rId29"/>
-    <sheet name="csv_road_mixer_lng" sheetId="68" r:id="rId30"/>
-    <sheet name="csv_bicycles_demand" sheetId="76" r:id="rId31"/>
+    <sheet name="csv_rail_electricity" sheetId="73" r:id="rId22"/>
+    <sheet name="csv_lng_mix" sheetId="75" r:id="rId23"/>
+    <sheet name="csv_network_gas_mix" sheetId="52" r:id="rId24"/>
+    <sheet name="csv_final_demand_road_greengas" sheetId="70" r:id="rId25"/>
+    <sheet name="csv_final_demand_natural_gas" sheetId="63" r:id="rId26"/>
+    <sheet name="csv_shipping_mixer_lng" sheetId="67" r:id="rId27"/>
+    <sheet name="csv_shipping_mixer_diesel" sheetId="69" r:id="rId28"/>
+    <sheet name="csv_road_mixer_lng" sheetId="68" r:id="rId29"/>
+    <sheet name="csv_bicycles_demand" sheetId="76" r:id="rId30"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId31"/>
     <externalReference r:id="rId32"/>
   </externalReferences>
   <definedNames>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="516">
   <si>
     <t>Changelog</t>
   </si>
@@ -1409,9 +1409,6 @@
     <t>Diesel rail</t>
   </si>
   <si>
-    <t>Coal rail</t>
-  </si>
-  <si>
     <t>Percentage of electricity delivered to trams/metro</t>
   </si>
   <si>
@@ -1427,12 +1424,6 @@
     <t>Percentage of diesel delivered to freight trains</t>
   </si>
   <si>
-    <t>Percentage of coal delivered to passenger trains</t>
-  </si>
-  <si>
-    <t>Percentage of coal delivered to freight trains</t>
-  </si>
-  <si>
     <t>Percentage of electricity delivered to bicycles</t>
   </si>
   <si>
@@ -1493,15 +1484,6 @@
     <t>transport_passenger_tram_using_electricity</t>
   </si>
   <si>
-    <t>transport_rail_mixer_coal_parent_share</t>
-  </si>
-  <si>
-    <t>transport_passenger_train_using_coal</t>
-  </si>
-  <si>
-    <t>transport_freight_train_using_coal</t>
-  </si>
-  <si>
     <t>transport_truck_using_lng</t>
   </si>
   <si>
@@ -1593,12 +1575,6 @@
   </si>
   <si>
     <t>Percentage_of_diesel_delivered_to_freight_trains</t>
-  </si>
-  <si>
-    <t>Percentage_of_coal_delivered_to_passenger_trains</t>
-  </si>
-  <si>
-    <t>Percentage_of_coal_delivered_to_freight_trains</t>
   </si>
   <si>
     <t>Percentage_of_gasoline_mix_delivered_to_motorbikes</t>
@@ -1689,6 +1665,7 @@
       <sz val="16"/>
       <color theme="3"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1703,6 +1680,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1710,11 +1688,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1722,6 +1702,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1758,6 +1739,7 @@
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1765,6 +1747,7 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1778,6 +1761,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1796,11 +1780,13 @@
       <sz val="12"/>
       <color theme="3"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1815,18 +1801,21 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1834,6 +1823,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1841,34 +1831,40 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -5075,19 +5071,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5102,28 +5107,19 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1728">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -8824,6 +8820,28 @@
     <sheetNames>
       <sheetName val="Cover sheet"/>
       <sheetName val="Dashboard"/>
+      <sheetName val="analysis_manager"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="export_data_button"/>
+      <definedName name="import_data_button"/>
+      <definedName name="select_dashboard_values"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover sheet"/>
+      <sheetName val="Dashboard"/>
     </sheetNames>
     <definedNames>
       <definedName name="export_data_button"/>
@@ -9543,7 +9561,7 @@
       <c r="B13" s="161"/>
       <c r="C13" s="205"/>
       <c r="D13" s="142" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E13" s="208">
         <f>Dashboard!E35</f>
@@ -9558,7 +9576,7 @@
       <c r="B14" s="161"/>
       <c r="C14" s="205"/>
       <c r="D14" s="142" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E14" s="208">
         <f>Dashboard!E37</f>
@@ -9573,7 +9591,7 @@
       <c r="B15" s="161"/>
       <c r="C15" s="205"/>
       <c r="D15" s="142" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E15" s="208">
         <f>Dashboard!E36</f>
@@ -9627,7 +9645,7 @@
       <c r="B19" s="161"/>
       <c r="C19" s="205"/>
       <c r="D19" s="142" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E19" s="208">
         <f>Dashboard!E26</f>
@@ -9642,7 +9660,7 @@
       <c r="B20" s="161"/>
       <c r="C20" s="205"/>
       <c r="D20" s="142" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E20" s="208">
         <f>Dashboard!E27</f>
@@ -9696,7 +9714,7 @@
       <c r="B24" s="161"/>
       <c r="C24" s="205"/>
       <c r="D24" s="142" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E24" s="208">
         <f>Dashboard!E31</f>
@@ -9750,7 +9768,7 @@
       <c r="B28" s="161"/>
       <c r="C28" s="205"/>
       <c r="D28" s="142" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E28" s="208">
         <f>Dashboard!E47</f>
@@ -9771,7 +9789,7 @@
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="161"/>
       <c r="C30" s="205" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D30" s="142" t="s">
         <v>303</v>
@@ -9789,7 +9807,7 @@
       <c r="B31" s="343"/>
       <c r="C31" s="355"/>
       <c r="D31" s="356" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E31" s="346">
         <f>Dashboard!E43</f>
@@ -9815,7 +9833,7 @@
         <v>108</v>
       </c>
       <c r="D33" s="349" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E33" s="347">
         <f>Dashboard!E67</f>
@@ -9831,7 +9849,7 @@
       <c r="B34" s="161"/>
       <c r="C34" s="205"/>
       <c r="D34" s="349" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E34" s="347">
         <f>Dashboard!E68</f>
@@ -9847,7 +9865,7 @@
       <c r="B35" s="161"/>
       <c r="C35" s="205"/>
       <c r="D35" s="18" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E35" s="347">
         <f>Dashboard!E69</f>
@@ -9873,7 +9891,7 @@
         <v>204</v>
       </c>
       <c r="D37" s="349" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E37" s="347">
         <f>Dashboard!E72</f>
@@ -9888,7 +9906,7 @@
       <c r="B38" s="31"/>
       <c r="C38" s="205"/>
       <c r="D38" s="18" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E38" s="347">
         <f>Dashboard!E73</f>
@@ -9914,15 +9932,15 @@
         <v>200</v>
       </c>
       <c r="D40" s="349" t="s">
-        <v>458</v>
-      </c>
-      <c r="E40" s="347">
-        <f>Dashboard!E76</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="144">
+        <v>455</v>
+      </c>
+      <c r="E40" s="347" t="e">
+        <f>Dashboard!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F40" s="144" t="e">
         <f>E40</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="G40" s="239"/>
     </row>
@@ -9930,15 +9948,15 @@
       <c r="B41" s="44"/>
       <c r="C41" s="350"/>
       <c r="D41" s="351" t="s">
-        <v>459</v>
-      </c>
-      <c r="E41" s="352">
-        <f>Dashboard!E77</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="353">
+        <v>456</v>
+      </c>
+      <c r="E41" s="352" t="e">
+        <f>Dashboard!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F41" s="353" t="e">
         <f>E41</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -10540,18 +10558,18 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B4" s="391" t="s">
+      <c r="B4" s="392" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="392"/>
-      <c r="D4" s="393"/>
+      <c r="C4" s="393"/>
+      <c r="D4" s="394"/>
     </row>
     <row r="5" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="394" t="s">
+      <c r="B5" s="395" t="s">
         <v>371</v>
       </c>
-      <c r="C5" s="395"/>
-      <c r="D5" s="396"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="397"/>
     </row>
     <row r="6" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:28" x14ac:dyDescent="0.2">
@@ -10570,20 +10588,20 @@
       <c r="L7" s="262"/>
       <c r="M7" s="262"/>
       <c r="N7" s="262"/>
-      <c r="O7" s="397"/>
-      <c r="P7" s="398"/>
-      <c r="Q7" s="398"/>
-      <c r="R7" s="398"/>
-      <c r="S7" s="398"/>
-      <c r="T7" s="398"/>
+      <c r="O7" s="398"/>
+      <c r="P7" s="399"/>
+      <c r="Q7" s="399"/>
+      <c r="R7" s="399"/>
+      <c r="S7" s="399"/>
+      <c r="T7" s="399"/>
       <c r="U7" s="236"/>
       <c r="V7" s="243"/>
       <c r="W7" s="236"/>
       <c r="X7" s="236"/>
-      <c r="Y7" s="401"/>
-      <c r="Z7" s="401"/>
-      <c r="AA7" s="401"/>
-      <c r="AB7" s="402"/>
+      <c r="Y7" s="378"/>
+      <c r="Z7" s="378"/>
+      <c r="AA7" s="378"/>
+      <c r="AB7" s="379"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" s="36"/>
@@ -10599,20 +10617,20 @@
       <c r="L8" s="239"/>
       <c r="M8" s="239"/>
       <c r="N8" s="239"/>
-      <c r="O8" s="384"/>
-      <c r="P8" s="382"/>
-      <c r="Q8" s="382"/>
-      <c r="R8" s="382"/>
-      <c r="S8" s="382"/>
-      <c r="T8" s="382"/>
+      <c r="O8" s="400"/>
+      <c r="P8" s="384"/>
+      <c r="Q8" s="384"/>
+      <c r="R8" s="384"/>
+      <c r="S8" s="384"/>
+      <c r="T8" s="384"/>
       <c r="U8" s="234"/>
       <c r="V8" s="244"/>
       <c r="W8" s="234"/>
       <c r="X8" s="234"/>
-      <c r="Y8" s="403"/>
-      <c r="Z8" s="403"/>
-      <c r="AA8" s="403"/>
-      <c r="AB8" s="404"/>
+      <c r="Y8" s="380"/>
+      <c r="Z8" s="380"/>
+      <c r="AA8" s="380"/>
+      <c r="AB8" s="381"/>
     </row>
     <row r="9" spans="2:28" ht="48" x14ac:dyDescent="0.2">
       <c r="B9" s="111" t="s">
@@ -10654,26 +10672,26 @@
       <c r="N9" s="265" t="s">
         <v>253</v>
       </c>
-      <c r="O9" s="399" t="s">
+      <c r="O9" s="401" t="s">
         <v>311</v>
       </c>
-      <c r="P9" s="400"/>
-      <c r="Q9" s="400"/>
-      <c r="R9" s="400"/>
-      <c r="S9" s="400"/>
-      <c r="T9" s="400"/>
+      <c r="P9" s="402"/>
+      <c r="Q9" s="402"/>
+      <c r="R9" s="402"/>
+      <c r="S9" s="402"/>
+      <c r="T9" s="402"/>
       <c r="U9" s="242"/>
       <c r="V9" s="245" t="s">
         <v>89</v>
       </c>
       <c r="W9" s="58"/>
       <c r="X9" s="58"/>
-      <c r="Y9" s="380" t="s">
+      <c r="Y9" s="382" t="s">
         <v>311</v>
       </c>
-      <c r="Z9" s="380"/>
-      <c r="AA9" s="380"/>
-      <c r="AB9" s="381"/>
+      <c r="Z9" s="382"/>
+      <c r="AA9" s="382"/>
+      <c r="AB9" s="383"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" s="230"/>
@@ -10689,20 +10707,20 @@
       <c r="L10" s="231"/>
       <c r="M10" s="231"/>
       <c r="N10" s="232"/>
-      <c r="O10" s="405"/>
-      <c r="P10" s="406"/>
-      <c r="Q10" s="406"/>
-      <c r="R10" s="406"/>
-      <c r="S10" s="406"/>
-      <c r="T10" s="406"/>
-      <c r="U10" s="406"/>
+      <c r="O10" s="388"/>
+      <c r="P10" s="389"/>
+      <c r="Q10" s="389"/>
+      <c r="R10" s="389"/>
+      <c r="S10" s="389"/>
+      <c r="T10" s="389"/>
+      <c r="U10" s="389"/>
       <c r="V10" s="248"/>
       <c r="W10" s="234"/>
       <c r="X10" s="234"/>
-      <c r="Y10" s="382"/>
-      <c r="Z10" s="382"/>
-      <c r="AA10" s="382"/>
-      <c r="AB10" s="383"/>
+      <c r="Y10" s="384"/>
+      <c r="Z10" s="384"/>
+      <c r="AA10" s="384"/>
+      <c r="AB10" s="385"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="114" t="s">
@@ -10755,20 +10773,20 @@
       <c r="N11" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O11" s="407"/>
-      <c r="P11" s="408"/>
-      <c r="Q11" s="408"/>
-      <c r="R11" s="408"/>
-      <c r="S11" s="408"/>
-      <c r="T11" s="408"/>
-      <c r="U11" s="408"/>
+      <c r="O11" s="390"/>
+      <c r="P11" s="391"/>
+      <c r="Q11" s="391"/>
+      <c r="R11" s="391"/>
+      <c r="S11" s="391"/>
+      <c r="T11" s="391"/>
+      <c r="U11" s="391"/>
       <c r="V11" s="247"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="382"/>
-      <c r="Z11" s="382"/>
-      <c r="AA11" s="382"/>
-      <c r="AB11" s="383"/>
+      <c r="Y11" s="384"/>
+      <c r="Z11" s="384"/>
+      <c r="AA11" s="384"/>
+      <c r="AB11" s="385"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B12" s="114" t="s">
@@ -10821,20 +10839,20 @@
       <c r="N12" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O12" s="389"/>
-      <c r="P12" s="390"/>
-      <c r="Q12" s="390"/>
-      <c r="R12" s="390"/>
-      <c r="S12" s="390"/>
-      <c r="T12" s="390"/>
-      <c r="U12" s="390"/>
+      <c r="O12" s="386"/>
+      <c r="P12" s="387"/>
+      <c r="Q12" s="387"/>
+      <c r="R12" s="387"/>
+      <c r="S12" s="387"/>
+      <c r="T12" s="387"/>
+      <c r="U12" s="387"/>
       <c r="V12" s="247"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="382"/>
-      <c r="Z12" s="382"/>
-      <c r="AA12" s="382"/>
-      <c r="AB12" s="383"/>
+      <c r="Y12" s="384"/>
+      <c r="Z12" s="384"/>
+      <c r="AA12" s="384"/>
+      <c r="AB12" s="385"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B13" s="114" t="s">
@@ -10887,20 +10905,20 @@
       <c r="N13" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O13" s="389"/>
-      <c r="P13" s="390"/>
-      <c r="Q13" s="390"/>
-      <c r="R13" s="390"/>
-      <c r="S13" s="390"/>
-      <c r="T13" s="390"/>
-      <c r="U13" s="390"/>
+      <c r="O13" s="386"/>
+      <c r="P13" s="387"/>
+      <c r="Q13" s="387"/>
+      <c r="R13" s="387"/>
+      <c r="S13" s="387"/>
+      <c r="T13" s="387"/>
+      <c r="U13" s="387"/>
       <c r="V13" s="247"/>
       <c r="W13" s="234"/>
       <c r="X13" s="234"/>
-      <c r="Y13" s="382"/>
-      <c r="Z13" s="382"/>
-      <c r="AA13" s="382"/>
-      <c r="AB13" s="383"/>
+      <c r="Y13" s="384"/>
+      <c r="Z13" s="384"/>
+      <c r="AA13" s="384"/>
+      <c r="AB13" s="385"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B14" s="114" t="s">
@@ -10942,22 +10960,22 @@
       <c r="N14" s="259" t="s">
         <v>287</v>
       </c>
-      <c r="O14" s="389" t="s">
+      <c r="O14" s="386" t="s">
         <v>373</v>
       </c>
-      <c r="P14" s="390"/>
-      <c r="Q14" s="390"/>
-      <c r="R14" s="390"/>
-      <c r="S14" s="390"/>
-      <c r="T14" s="390"/>
-      <c r="U14" s="390"/>
+      <c r="P14" s="387"/>
+      <c r="Q14" s="387"/>
+      <c r="R14" s="387"/>
+      <c r="S14" s="387"/>
+      <c r="T14" s="387"/>
+      <c r="U14" s="387"/>
       <c r="V14" s="247"/>
       <c r="W14" s="115"/>
       <c r="X14" s="115"/>
-      <c r="Y14" s="382"/>
-      <c r="Z14" s="382"/>
-      <c r="AA14" s="382"/>
-      <c r="AB14" s="383"/>
+      <c r="Y14" s="384"/>
+      <c r="Z14" s="384"/>
+      <c r="AA14" s="384"/>
+      <c r="AB14" s="385"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B15" s="114" t="s">
@@ -11010,20 +11028,20 @@
       <c r="N15" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O15" s="389"/>
-      <c r="P15" s="390"/>
-      <c r="Q15" s="390"/>
-      <c r="R15" s="390"/>
-      <c r="S15" s="390"/>
-      <c r="T15" s="390"/>
-      <c r="U15" s="390"/>
+      <c r="O15" s="386"/>
+      <c r="P15" s="387"/>
+      <c r="Q15" s="387"/>
+      <c r="R15" s="387"/>
+      <c r="S15" s="387"/>
+      <c r="T15" s="387"/>
+      <c r="U15" s="387"/>
       <c r="V15" s="250"/>
       <c r="W15" s="58"/>
       <c r="X15" s="58"/>
-      <c r="Y15" s="380"/>
-      <c r="Z15" s="380"/>
-      <c r="AA15" s="380"/>
-      <c r="AB15" s="381"/>
+      <c r="Y15" s="382"/>
+      <c r="Z15" s="382"/>
+      <c r="AA15" s="382"/>
+      <c r="AB15" s="383"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B16" s="113" t="s">
@@ -11066,15 +11084,15 @@
       <c r="N16" s="225" t="s">
         <v>287</v>
       </c>
-      <c r="O16" s="389" t="s">
+      <c r="O16" s="386" t="s">
         <v>374</v>
       </c>
-      <c r="P16" s="390"/>
-      <c r="Q16" s="390"/>
-      <c r="R16" s="390"/>
-      <c r="S16" s="390"/>
-      <c r="T16" s="390"/>
-      <c r="U16" s="390"/>
+      <c r="P16" s="387"/>
+      <c r="Q16" s="387"/>
+      <c r="R16" s="387"/>
+      <c r="S16" s="387"/>
+      <c r="T16" s="387"/>
+      <c r="U16" s="387"/>
       <c r="V16" s="246" t="s">
         <v>361</v>
       </c>
@@ -11099,13 +11117,13 @@
       <c r="L17" s="219"/>
       <c r="M17" s="219"/>
       <c r="N17" s="219"/>
-      <c r="O17" s="384"/>
-      <c r="P17" s="382"/>
-      <c r="Q17" s="382"/>
-      <c r="R17" s="382"/>
-      <c r="S17" s="382"/>
-      <c r="T17" s="382"/>
-      <c r="U17" s="382"/>
+      <c r="O17" s="400"/>
+      <c r="P17" s="384"/>
+      <c r="Q17" s="384"/>
+      <c r="R17" s="384"/>
+      <c r="S17" s="384"/>
+      <c r="T17" s="384"/>
+      <c r="U17" s="384"/>
       <c r="V17" s="247"/>
       <c r="W17" s="251" t="s">
         <v>364</v>
@@ -11157,15 +11175,15 @@
         <f>'Corrected energy balance step 2'!BN90</f>
         <v>0</v>
       </c>
-      <c r="O18" s="387" t="s">
+      <c r="O18" s="407" t="s">
         <v>312</v>
       </c>
-      <c r="P18" s="388"/>
-      <c r="Q18" s="388"/>
-      <c r="R18" s="388"/>
-      <c r="S18" s="388"/>
-      <c r="T18" s="388"/>
-      <c r="U18" s="388"/>
+      <c r="P18" s="408"/>
+      <c r="Q18" s="408"/>
+      <c r="R18" s="408"/>
+      <c r="S18" s="408"/>
+      <c r="T18" s="408"/>
+      <c r="U18" s="408"/>
       <c r="V18" s="247"/>
       <c r="AB18" s="235"/>
     </row>
@@ -11183,13 +11201,13 @@
       <c r="L19" s="221"/>
       <c r="M19" s="221"/>
       <c r="N19" s="221"/>
-      <c r="O19" s="385"/>
-      <c r="P19" s="386"/>
-      <c r="Q19" s="386"/>
-      <c r="R19" s="386"/>
-      <c r="S19" s="386"/>
-      <c r="T19" s="386"/>
-      <c r="U19" s="386"/>
+      <c r="O19" s="405"/>
+      <c r="P19" s="406"/>
+      <c r="Q19" s="406"/>
+      <c r="R19" s="406"/>
+      <c r="S19" s="406"/>
+      <c r="T19" s="406"/>
+      <c r="U19" s="406"/>
       <c r="V19" s="247"/>
       <c r="W19" s="201" t="s">
         <v>365</v>
@@ -11217,13 +11235,13 @@
       <c r="L20" s="263"/>
       <c r="M20" s="263"/>
       <c r="N20" s="263"/>
-      <c r="O20" s="384"/>
-      <c r="P20" s="382"/>
-      <c r="Q20" s="382"/>
-      <c r="R20" s="382"/>
-      <c r="S20" s="382"/>
-      <c r="T20" s="382"/>
-      <c r="U20" s="382"/>
+      <c r="O20" s="400"/>
+      <c r="P20" s="384"/>
+      <c r="Q20" s="384"/>
+      <c r="R20" s="384"/>
+      <c r="S20" s="384"/>
+      <c r="T20" s="384"/>
+      <c r="U20" s="384"/>
       <c r="V20" s="247"/>
       <c r="W20" s="201" t="s">
         <v>366</v>
@@ -11288,13 +11306,13 @@
       <c r="N21" s="227" t="s">
         <v>287</v>
       </c>
-      <c r="O21" s="385"/>
-      <c r="P21" s="386"/>
-      <c r="Q21" s="386"/>
-      <c r="R21" s="386"/>
-      <c r="S21" s="386"/>
-      <c r="T21" s="386"/>
-      <c r="U21" s="386"/>
+      <c r="O21" s="405"/>
+      <c r="P21" s="406"/>
+      <c r="Q21" s="406"/>
+      <c r="R21" s="406"/>
+      <c r="S21" s="406"/>
+      <c r="T21" s="406"/>
+      <c r="U21" s="406"/>
       <c r="V21" s="247"/>
       <c r="W21" s="234"/>
       <c r="X21" s="234"/>
@@ -11344,13 +11362,13 @@
         <f>N18</f>
         <v>0</v>
       </c>
-      <c r="O22" s="385"/>
-      <c r="P22" s="386"/>
-      <c r="Q22" s="386"/>
-      <c r="R22" s="386"/>
-      <c r="S22" s="386"/>
-      <c r="T22" s="386"/>
-      <c r="U22" s="386"/>
+      <c r="O22" s="405"/>
+      <c r="P22" s="406"/>
+      <c r="Q22" s="406"/>
+      <c r="R22" s="406"/>
+      <c r="S22" s="406"/>
+      <c r="T22" s="406"/>
+      <c r="U22" s="406"/>
       <c r="V22" s="247"/>
       <c r="W22" s="234"/>
       <c r="X22" s="234"/>
@@ -11386,13 +11404,13 @@
       <c r="L23" s="266"/>
       <c r="M23" s="266"/>
       <c r="N23" s="266"/>
-      <c r="O23" s="378"/>
-      <c r="P23" s="379"/>
-      <c r="Q23" s="379"/>
-      <c r="R23" s="379"/>
-      <c r="S23" s="379"/>
-      <c r="T23" s="379"/>
-      <c r="U23" s="379"/>
+      <c r="O23" s="403"/>
+      <c r="P23" s="404"/>
+      <c r="Q23" s="404"/>
+      <c r="R23" s="404"/>
+      <c r="S23" s="404"/>
+      <c r="T23" s="404"/>
+      <c r="U23" s="404"/>
       <c r="V23" s="249"/>
       <c r="W23" s="237"/>
       <c r="X23" s="237"/>
@@ -11418,14 +11436,31 @@
       <c r="V24" s="234"/>
       <c r="W24" s="115"/>
       <c r="X24" s="115"/>
-      <c r="Y24" s="382"/>
-      <c r="Z24" s="382"/>
-      <c r="AA24" s="382"/>
-      <c r="AB24" s="382"/>
+      <c r="Y24" s="384"/>
+      <c r="Z24" s="384"/>
+      <c r="AA24" s="384"/>
+      <c r="AB24" s="384"/>
       <c r="AC24" s="234"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="O23:U23"/>
+    <mergeCell ref="Y15:AB15"/>
+    <mergeCell ref="Y24:AB24"/>
+    <mergeCell ref="Y13:AB13"/>
+    <mergeCell ref="O20:U20"/>
+    <mergeCell ref="O21:U21"/>
+    <mergeCell ref="O22:U22"/>
+    <mergeCell ref="O18:U18"/>
+    <mergeCell ref="O19:U19"/>
+    <mergeCell ref="O15:U15"/>
+    <mergeCell ref="O16:U16"/>
+    <mergeCell ref="O17:U17"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="O8:T8"/>
+    <mergeCell ref="O9:T9"/>
     <mergeCell ref="Y7:AB7"/>
     <mergeCell ref="Y8:AB8"/>
     <mergeCell ref="Y9:AB9"/>
@@ -11438,23 +11473,6 @@
     <mergeCell ref="O10:U10"/>
     <mergeCell ref="O11:U11"/>
     <mergeCell ref="O12:U12"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="O8:T8"/>
-    <mergeCell ref="O9:T9"/>
-    <mergeCell ref="O23:U23"/>
-    <mergeCell ref="Y15:AB15"/>
-    <mergeCell ref="Y24:AB24"/>
-    <mergeCell ref="Y13:AB13"/>
-    <mergeCell ref="O20:U20"/>
-    <mergeCell ref="O21:U21"/>
-    <mergeCell ref="O22:U22"/>
-    <mergeCell ref="O18:U18"/>
-    <mergeCell ref="O19:U19"/>
-    <mergeCell ref="O15:U15"/>
-    <mergeCell ref="O16:U16"/>
-    <mergeCell ref="O17:U17"/>
   </mergeCells>
   <conditionalFormatting sqref="X19:X20">
     <cfRule type="duplicateValues" dxfId="2" priority="5"/>
@@ -11815,7 +11833,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B5" s="155">
         <f>'Technology Shares'!F13</f>
@@ -11824,7 +11842,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B6" s="155">
         <f>'Technology Shares'!F14</f>
@@ -11833,7 +11851,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="B7" s="155">
         <f>'Technology Shares'!F15</f>
@@ -11916,7 +11934,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B5" s="155">
         <f>'Technology Shares'!F19</f>
@@ -11935,7 +11953,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="B6" s="155">
         <f>'Technology Shares'!F20</f>
@@ -12244,7 +12262,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B5" s="155">
         <f>'Technology Shares'!F24</f>
@@ -12276,7 +12294,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -12289,7 +12307,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B3" s="155">
         <f>'Technology Shares'!F37</f>
@@ -12298,7 +12316,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B4" s="155">
         <f>'Technology Shares'!F38</f>
@@ -12321,86 +12339,6 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>475</v>
-      </c>
-      <c r="B3" s="155">
-        <f>'Technology Shares'!F40</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="155"/>
-      <c r="E3" s="155"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>476</v>
-      </c>
-      <c r="B4" s="155">
-        <f>'Technology Shares'!F41</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="155"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="155"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="155"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="358"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D8" s="358"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12420,7 +12358,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -12433,7 +12371,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B3" s="155">
         <f>'Technology Shares'!F33</f>
@@ -12446,7 +12384,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B4" s="155">
         <f>'Technology Shares'!F34</f>
@@ -12458,7 +12396,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B5" s="155">
         <f>'Technology Shares'!F35</f>
@@ -12486,7 +12424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12505,7 +12443,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C1" s="155"/>
     </row>
@@ -12520,7 +12458,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B3" s="155">
         <f>'Technology Shares'!F30</f>
@@ -12533,7 +12471,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B4" s="155">
         <f>'Technology Shares'!F31</f>
@@ -12551,7 +12489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12601,7 +12539,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B5" s="155">
         <f>'Technology Shares'!F28</f>
@@ -12614,7 +12552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12668,7 +12606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12719,7 +12657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12775,7 +12713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -12851,6 +12789,62 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="330" t="s">
+        <v>381</v>
+      </c>
+      <c r="B3" s="317">
+        <f>'Fuelling shares'!E29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="330" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" s="317">
+        <f xml:space="preserve"> 'Fuelling shares'!E30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="133"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
@@ -12959,62 +12953,6 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="39.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="330" t="s">
-        <v>381</v>
-      </c>
-      <c r="B3" s="317">
-        <f>'Fuelling shares'!E29</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="330" t="s">
-        <v>421</v>
-      </c>
-      <c r="B4" s="317">
-        <f xml:space="preserve"> 'Fuelling shares'!E30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="133"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13025,7 +12963,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -13033,12 +12971,12 @@
         <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="B3" s="370">
         <f>Dashboard!E53</f>
@@ -14369,10 +14307,10 @@
   <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Y78"/>
+  <dimension ref="A1:Y75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14565,7 +14503,7 @@
       </c>
       <c r="D11" s="239"/>
       <c r="E11" s="205" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="F11" s="338"/>
       <c r="G11" s="22" t="s">
@@ -14879,7 +14817,7 @@
       <c r="M24" s="50"/>
       <c r="N24" s="240"/>
       <c r="O24" s="172" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="P24" s="162"/>
     </row>
@@ -14902,7 +14840,7 @@
       <c r="M25" s="50"/>
       <c r="N25" s="240"/>
       <c r="O25" s="172" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="P25" s="162"/>
     </row>
@@ -14925,14 +14863,14 @@
       <c r="M26" s="50"/>
       <c r="N26" s="240"/>
       <c r="O26" s="172" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="P26" s="162"/>
     </row>
     <row r="27" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="31"/>
       <c r="C27" s="239" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="D27" s="239" t="s">
         <v>320</v>
@@ -14948,7 +14886,7 @@
       <c r="M27" s="50"/>
       <c r="N27" s="240"/>
       <c r="O27" s="172" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="P27" s="162"/>
     </row>
@@ -14988,7 +14926,7 @@
       <c r="M29" s="50"/>
       <c r="N29" s="240"/>
       <c r="O29" s="172" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="P29" s="162"/>
     </row>
@@ -15011,7 +14949,7 @@
       <c r="M30" s="50"/>
       <c r="N30" s="240"/>
       <c r="O30" s="172" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="P30" s="162"/>
     </row>
@@ -15034,7 +14972,7 @@
       <c r="M31" s="50"/>
       <c r="N31" s="240"/>
       <c r="O31" s="172" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="P31" s="162"/>
     </row>
@@ -15074,7 +15012,7 @@
       <c r="M33" s="50"/>
       <c r="N33" s="240"/>
       <c r="O33" s="172" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="P33" s="162"/>
     </row>
@@ -15097,7 +15035,7 @@
       <c r="M34" s="50"/>
       <c r="N34" s="240"/>
       <c r="O34" s="172" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="P34" s="162"/>
     </row>
@@ -15120,14 +15058,14 @@
       <c r="M35" s="50"/>
       <c r="N35" s="240"/>
       <c r="O35" s="172" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="P35" s="162"/>
     </row>
     <row r="36" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="31"/>
       <c r="C36" s="239" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="D36" s="239" t="s">
         <v>320</v>
@@ -15143,14 +15081,14 @@
       <c r="M36" s="50"/>
       <c r="N36" s="240"/>
       <c r="O36" s="172" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="P36" s="162"/>
     </row>
     <row r="37" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="31"/>
       <c r="C37" s="239" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D37" s="239" t="s">
         <v>320</v>
@@ -15166,7 +15104,7 @@
       <c r="M37" s="50"/>
       <c r="N37" s="240"/>
       <c r="O37" s="172" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="P37" s="162"/>
     </row>
@@ -15206,7 +15144,7 @@
       <c r="M39" s="50"/>
       <c r="N39" s="240"/>
       <c r="O39" s="172" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="P39" s="162"/>
     </row>
@@ -15229,7 +15167,7 @@
       <c r="M40" s="50"/>
       <c r="N40" s="240"/>
       <c r="O40" s="172" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="P40" s="162"/>
     </row>
@@ -15269,14 +15207,14 @@
       <c r="M42" s="50"/>
       <c r="N42" s="240"/>
       <c r="O42" s="172" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="P42" s="162"/>
     </row>
     <row r="43" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="31"/>
       <c r="C43" s="239" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D43" s="239" t="s">
         <v>320</v>
@@ -15292,7 +15230,7 @@
       <c r="M43" s="50"/>
       <c r="N43" s="240"/>
       <c r="O43" s="172" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="P43" s="162"/>
     </row>
@@ -15332,7 +15270,7 @@
       <c r="M45" s="50"/>
       <c r="N45" s="240"/>
       <c r="O45" s="172" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="P45" s="162"/>
     </row>
@@ -15355,7 +15293,7 @@
       <c r="M46" s="50"/>
       <c r="N46" s="240"/>
       <c r="O46" s="172" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="P46" s="162"/>
     </row>
@@ -15378,7 +15316,7 @@
       <c r="M47" s="50"/>
       <c r="N47" s="240"/>
       <c r="O47" s="172" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="P47" s="162"/>
     </row>
@@ -15442,7 +15380,7 @@
       <c r="M50" s="50"/>
       <c r="N50" s="240"/>
       <c r="O50" s="172" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="P50" s="162"/>
     </row>
@@ -15465,7 +15403,7 @@
       <c r="M51" s="50"/>
       <c r="N51" s="240"/>
       <c r="O51" s="172" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="P51" s="162"/>
     </row>
@@ -15489,10 +15427,10 @@
     <row r="53" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="31"/>
       <c r="C53" s="239" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="D53" s="239" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E53" s="23"/>
       <c r="F53" s="239"/>
@@ -15505,7 +15443,7 @@
       <c r="M53" s="50"/>
       <c r="N53" s="240"/>
       <c r="O53" s="172" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="P53" s="162"/>
     </row>
@@ -15605,7 +15543,7 @@
       <c r="M58" s="50"/>
       <c r="N58" s="240"/>
       <c r="O58" s="172" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="P58" s="162"/>
     </row>
@@ -15628,7 +15566,7 @@
       <c r="M59" s="50"/>
       <c r="N59" s="240"/>
       <c r="O59" s="172" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="P59" s="162"/>
     </row>
@@ -15692,7 +15630,7 @@
       <c r="M62" s="50"/>
       <c r="N62" s="240"/>
       <c r="O62" s="172" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="P62" s="162"/>
     </row>
@@ -15715,7 +15653,7 @@
       <c r="M63" s="50"/>
       <c r="N63" s="240"/>
       <c r="O63" s="172" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="P63" s="162"/>
     </row>
@@ -15784,7 +15722,7 @@
     <row r="67" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="31"/>
       <c r="C67" s="239" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D67" s="239" t="s">
         <v>320</v>
@@ -15800,7 +15738,7 @@
       <c r="M67" s="239"/>
       <c r="N67" s="366"/>
       <c r="O67" s="172" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="P67" s="7"/>
       <c r="Q67" s="19"/>
@@ -15816,7 +15754,7 @@
     <row r="68" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B68" s="31"/>
       <c r="C68" s="239" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D68" s="239" t="s">
         <v>320</v>
@@ -15832,7 +15770,7 @@
       <c r="M68" s="239"/>
       <c r="N68" s="366"/>
       <c r="O68" s="172" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="P68" s="7"/>
       <c r="Q68" s="19"/>
@@ -15848,7 +15786,7 @@
     <row r="69" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" s="31"/>
       <c r="C69" s="239" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D69" s="239" t="s">
         <v>320</v>
@@ -15864,7 +15802,7 @@
       <c r="M69" s="239"/>
       <c r="N69" s="366"/>
       <c r="O69" s="172" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="P69" s="7"/>
       <c r="Q69" s="19"/>
@@ -15939,7 +15877,7 @@
     <row r="72" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="31"/>
       <c r="C72" s="239" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D72" s="239" t="s">
         <v>320</v>
@@ -15955,7 +15893,7 @@
       <c r="M72" s="239"/>
       <c r="N72" s="366"/>
       <c r="O72" s="172" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="P72" s="7"/>
       <c r="Q72" s="19"/>
@@ -15971,7 +15909,7 @@
     <row r="73" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B73" s="31"/>
       <c r="C73" s="239" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D73" s="239" t="s">
         <v>320</v>
@@ -15987,7 +15925,7 @@
       <c r="M73" s="239"/>
       <c r="N73" s="366"/>
       <c r="O73" s="172" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="P73" s="7"/>
       <c r="Q73" s="19"/>
@@ -16027,127 +15965,30 @@
       <c r="Y74" s="239"/>
     </row>
     <row r="75" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="31"/>
-      <c r="C75" s="239" t="s">
-        <v>446</v>
-      </c>
-      <c r="D75" s="239" t="s">
-        <v>293</v>
-      </c>
-      <c r="E75" s="362">
-        <f>'Fuel Aggregation'!C13</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="239"/>
-      <c r="G75" s="239"/>
-      <c r="H75" s="239"/>
-      <c r="I75" s="239"/>
-      <c r="J75" s="239"/>
-      <c r="K75" s="49"/>
-      <c r="L75" s="49"/>
-      <c r="M75" s="239"/>
-      <c r="N75" s="366"/>
-      <c r="O75" s="172"/>
-      <c r="P75" s="7"/>
-      <c r="Q75" s="19"/>
-      <c r="R75" s="239"/>
-      <c r="S75" s="239"/>
-      <c r="T75" s="239"/>
-      <c r="U75" s="239"/>
-      <c r="V75" s="239"/>
-      <c r="W75" s="239"/>
-      <c r="X75" s="239"/>
-      <c r="Y75" s="239"/>
-    </row>
-    <row r="76" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="31"/>
-      <c r="C76" s="239" t="s">
-        <v>452</v>
-      </c>
-      <c r="D76" s="239" t="s">
-        <v>320</v>
-      </c>
-      <c r="E76" s="342"/>
-      <c r="F76" s="239"/>
-      <c r="G76" s="239"/>
-      <c r="H76" s="239"/>
-      <c r="I76" s="23"/>
-      <c r="J76" s="239"/>
-      <c r="K76" s="49"/>
-      <c r="L76" s="49"/>
-      <c r="M76" s="239"/>
-      <c r="N76" s="366"/>
-      <c r="O76" s="172" t="s">
-        <v>508</v>
-      </c>
-      <c r="P76" s="7"/>
-      <c r="Q76" s="19"/>
-      <c r="R76" s="239"/>
-      <c r="S76" s="239"/>
-      <c r="T76" s="239"/>
-      <c r="U76" s="239"/>
-      <c r="V76" s="239"/>
-      <c r="W76" s="239"/>
-      <c r="X76" s="239"/>
-      <c r="Y76" s="239"/>
-    </row>
-    <row r="77" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="31"/>
-      <c r="C77" s="239" t="s">
-        <v>453</v>
-      </c>
-      <c r="D77" s="239" t="s">
-        <v>320</v>
-      </c>
-      <c r="E77" s="342"/>
-      <c r="F77" s="239"/>
-      <c r="G77" s="239"/>
-      <c r="H77" s="239"/>
-      <c r="I77" s="23"/>
-      <c r="J77" s="239"/>
-      <c r="K77" s="49"/>
-      <c r="L77" s="49"/>
-      <c r="M77" s="239"/>
-      <c r="N77" s="366"/>
-      <c r="O77" s="172" t="s">
-        <v>509</v>
-      </c>
-      <c r="P77" s="7"/>
-      <c r="Q77" s="19"/>
-      <c r="R77" s="239"/>
-      <c r="S77" s="239"/>
-      <c r="T77" s="239"/>
-      <c r="U77" s="239"/>
-      <c r="V77" s="239"/>
-      <c r="W77" s="239"/>
-      <c r="X77" s="239"/>
-      <c r="Y77" s="239"/>
-    </row>
-    <row r="78" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="44"/>
-      <c r="C78" s="63"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
-      <c r="F78" s="63"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="63"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="63"/>
-      <c r="K78" s="364"/>
-      <c r="L78" s="364"/>
-      <c r="M78" s="63"/>
-      <c r="N78" s="369"/>
-      <c r="O78" s="361"/>
-      <c r="P78" s="11"/>
-      <c r="Q78" s="20"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="10"/>
-      <c r="T78" s="10"/>
-      <c r="U78" s="10"/>
-      <c r="V78" s="10"/>
-      <c r="W78" s="10"/>
-      <c r="X78" s="10"/>
-      <c r="Y78" s="10"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="63"/>
+      <c r="F75" s="63"/>
+      <c r="G75" s="63"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="63"/>
+      <c r="J75" s="63"/>
+      <c r="K75" s="364"/>
+      <c r="L75" s="364"/>
+      <c r="M75" s="63"/>
+      <c r="N75" s="369"/>
+      <c r="O75" s="361"/>
+      <c r="P75" s="11"/>
+      <c r="Q75" s="20"/>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
+      <c r="U75" s="10"/>
+      <c r="V75" s="10"/>
+      <c r="W75" s="10"/>
+      <c r="X75" s="10"/>
+      <c r="Y75" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16179,7 +16020,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="9222" r:id="rId3" name="import_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!import_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!import_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -16202,7 +16043,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="9223" r:id="rId4" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!export_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!export_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -16225,7 +16066,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="9224" r:id="rId5" name="select_dashboard">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!select_dashboard_values">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!select_dashboard_values">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>

</xml_diff>

<commit_message>
published state of ETDataset on 1st of August  2018
</commit_message>
<xml_diff>
--- a/analyses/8_transport_analysis.xlsx
+++ b/analyses/8_transport_analysis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martlubben/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F0ADD1-36CB-A74F-8BA3-CB9531F20A97}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="891" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27920" windowHeight="16500" tabRatio="891" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -45,13 +46,12 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId31"/>
-    <externalReference r:id="rId32"/>
   </externalReferences>
   <definedNames>
     <definedName name="base_year">Dashboard!$E$12</definedName>
     <definedName name="country">Dashboard!$E$11</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1622,7 +1622,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
@@ -5071,28 +5071,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5107,19 +5098,28 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1728">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -6843,13 +6843,13 @@
     <cellStyle name="Hyperlink" xfId="1722" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1724" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1726" builtinId="8" hidden="1"/>
-    <cellStyle name="Input cel" xfId="1023"/>
+    <cellStyle name="Input cel" xfId="1023" xr:uid="{00000000-0005-0000-0000-0000B9060000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1011"/>
+    <cellStyle name="Normal 2" xfId="1011" xr:uid="{00000000-0005-0000-0000-0000BB060000}"/>
     <cellStyle name="Output" xfId="408" builtinId="21"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="1012"/>
-    <cellStyle name="Warning Text 3" xfId="1024"/>
+    <cellStyle name="Percent 2" xfId="1012" xr:uid="{00000000-0005-0000-0000-0000BE060000}"/>
+    <cellStyle name="Warning Text 3" xfId="1024" xr:uid="{00000000-0005-0000-0000-0000BF060000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -6916,6 +6916,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -6949,7 +6952,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="81" name="Rectangle 80"/>
+        <xdr:cNvPr id="81" name="Rectangle 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000051000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7024,7 +7033,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Rectangle 28"/>
+        <xdr:cNvPr id="29" name="Rectangle 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7087,7 +7102,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Rectangle 30"/>
+        <xdr:cNvPr id="31" name="Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7148,7 +7169,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="Rectangle 32"/>
+        <xdr:cNvPr id="33" name="Rectangle 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7211,7 +7238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="L-Shape 27"/>
+        <xdr:cNvPr id="28" name="L-Shape 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7275,7 +7308,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Rectangle 33"/>
+        <xdr:cNvPr id="34" name="Rectangle 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7428,7 +7467,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7495,7 +7540,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7551,7 +7602,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7601,7 +7658,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Connector 10"/>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -7651,7 +7714,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7707,7 +7776,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 18"/>
+        <xdr:cNvPr id="19" name="Rectangle 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7763,7 +7838,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectangle 21"/>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7847,7 +7928,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="24" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="7" idx="3"/>
           <a:endCxn id="62" idx="1"/>
@@ -7899,7 +7986,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="Rectangle 61"/>
+        <xdr:cNvPr id="62" name="Rectangle 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7960,7 +8053,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="152" name="Straight Arrow Connector 278"/>
+        <xdr:cNvPr id="152" name="Straight Arrow Connector 278">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000098000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="12" idx="3"/>
           <a:endCxn id="19" idx="1"/>
@@ -8010,7 +8109,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Straight Arrow Connector 278"/>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 278">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="19" idx="3"/>
           <a:endCxn id="52" idx="1"/>
@@ -8060,7 +8165,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Rectangle 38"/>
+        <xdr:cNvPr id="39" name="Rectangle 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8119,7 +8230,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Rectangle 50"/>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8175,7 +8292,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Rectangle 51"/>
+        <xdr:cNvPr id="52" name="Rectangle 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8231,7 +8354,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="Rectangle 59"/>
+        <xdr:cNvPr id="60" name="Rectangle 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8313,7 +8442,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="61" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="62" idx="3"/>
           <a:endCxn id="51" idx="1"/>
@@ -8363,7 +8498,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="68" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000044000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="52" idx="3"/>
           <a:endCxn id="60" idx="1"/>
@@ -8413,7 +8554,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Elbow Connector 23"/>
+        <xdr:cNvPr id="75" name="Elbow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="51" idx="3"/>
           <a:endCxn id="22" idx="1"/>
@@ -8463,7 +8610,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Straight Arrow Connector 77"/>
+        <xdr:cNvPr id="78" name="Straight Arrow Connector 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -8512,7 +8665,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Straight Arrow Connector 78"/>
+        <xdr:cNvPr id="79" name="Straight Arrow Connector 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="29" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -8561,7 +8720,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="Rectangle 79"/>
+        <xdr:cNvPr id="80" name="Rectangle 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000050000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8632,6 +8797,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s9222"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006240000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -8663,9 +8831,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>import data</a:t>
               </a:r>
@@ -8699,6 +8866,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s9223"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007240000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -8730,9 +8900,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>export to 'data/…/ouput' folder</a:t>
               </a:r>
@@ -8766,6 +8935,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s9224"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008240000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -8797,9 +8969,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>optional: load different Dashbord values</a:t>
               </a:r>
@@ -8831,26 +9002,6 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover sheet"/>
-      <sheetName val="Dashboard"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="export_data_button"/>
-      <definedName name="import_data_button"/>
-      <definedName name="select_dashboard_values"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9177,8 +9328,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:D38"/>
@@ -9438,8 +9589,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A2:G43"/>
@@ -9982,8 +10133,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:F45"/>
@@ -10514,8 +10665,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet11">
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:AO24"/>
@@ -10558,18 +10709,18 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B4" s="392" t="s">
+      <c r="B4" s="391" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="393"/>
-      <c r="D4" s="394"/>
+      <c r="C4" s="392"/>
+      <c r="D4" s="393"/>
     </row>
     <row r="5" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="395" t="s">
+      <c r="B5" s="394" t="s">
         <v>371</v>
       </c>
-      <c r="C5" s="396"/>
-      <c r="D5" s="397"/>
+      <c r="C5" s="395"/>
+      <c r="D5" s="396"/>
     </row>
     <row r="6" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:28" x14ac:dyDescent="0.2">
@@ -10588,20 +10739,20 @@
       <c r="L7" s="262"/>
       <c r="M7" s="262"/>
       <c r="N7" s="262"/>
-      <c r="O7" s="398"/>
-      <c r="P7" s="399"/>
-      <c r="Q7" s="399"/>
-      <c r="R7" s="399"/>
-      <c r="S7" s="399"/>
-      <c r="T7" s="399"/>
+      <c r="O7" s="397"/>
+      <c r="P7" s="398"/>
+      <c r="Q7" s="398"/>
+      <c r="R7" s="398"/>
+      <c r="S7" s="398"/>
+      <c r="T7" s="398"/>
       <c r="U7" s="236"/>
       <c r="V7" s="243"/>
       <c r="W7" s="236"/>
       <c r="X7" s="236"/>
-      <c r="Y7" s="378"/>
-      <c r="Z7" s="378"/>
-      <c r="AA7" s="378"/>
-      <c r="AB7" s="379"/>
+      <c r="Y7" s="401"/>
+      <c r="Z7" s="401"/>
+      <c r="AA7" s="401"/>
+      <c r="AB7" s="402"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" s="36"/>
@@ -10617,20 +10768,20 @@
       <c r="L8" s="239"/>
       <c r="M8" s="239"/>
       <c r="N8" s="239"/>
-      <c r="O8" s="400"/>
-      <c r="P8" s="384"/>
-      <c r="Q8" s="384"/>
-      <c r="R8" s="384"/>
-      <c r="S8" s="384"/>
-      <c r="T8" s="384"/>
+      <c r="O8" s="384"/>
+      <c r="P8" s="382"/>
+      <c r="Q8" s="382"/>
+      <c r="R8" s="382"/>
+      <c r="S8" s="382"/>
+      <c r="T8" s="382"/>
       <c r="U8" s="234"/>
       <c r="V8" s="244"/>
       <c r="W8" s="234"/>
       <c r="X8" s="234"/>
-      <c r="Y8" s="380"/>
-      <c r="Z8" s="380"/>
-      <c r="AA8" s="380"/>
-      <c r="AB8" s="381"/>
+      <c r="Y8" s="403"/>
+      <c r="Z8" s="403"/>
+      <c r="AA8" s="403"/>
+      <c r="AB8" s="404"/>
     </row>
     <row r="9" spans="2:28" ht="48" x14ac:dyDescent="0.2">
       <c r="B9" s="111" t="s">
@@ -10672,26 +10823,26 @@
       <c r="N9" s="265" t="s">
         <v>253</v>
       </c>
-      <c r="O9" s="401" t="s">
+      <c r="O9" s="399" t="s">
         <v>311</v>
       </c>
-      <c r="P9" s="402"/>
-      <c r="Q9" s="402"/>
-      <c r="R9" s="402"/>
-      <c r="S9" s="402"/>
-      <c r="T9" s="402"/>
+      <c r="P9" s="400"/>
+      <c r="Q9" s="400"/>
+      <c r="R9" s="400"/>
+      <c r="S9" s="400"/>
+      <c r="T9" s="400"/>
       <c r="U9" s="242"/>
       <c r="V9" s="245" t="s">
         <v>89</v>
       </c>
       <c r="W9" s="58"/>
       <c r="X9" s="58"/>
-      <c r="Y9" s="382" t="s">
+      <c r="Y9" s="380" t="s">
         <v>311</v>
       </c>
-      <c r="Z9" s="382"/>
-      <c r="AA9" s="382"/>
-      <c r="AB9" s="383"/>
+      <c r="Z9" s="380"/>
+      <c r="AA9" s="380"/>
+      <c r="AB9" s="381"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" s="230"/>
@@ -10707,20 +10858,20 @@
       <c r="L10" s="231"/>
       <c r="M10" s="231"/>
       <c r="N10" s="232"/>
-      <c r="O10" s="388"/>
-      <c r="P10" s="389"/>
-      <c r="Q10" s="389"/>
-      <c r="R10" s="389"/>
-      <c r="S10" s="389"/>
-      <c r="T10" s="389"/>
-      <c r="U10" s="389"/>
+      <c r="O10" s="405"/>
+      <c r="P10" s="406"/>
+      <c r="Q10" s="406"/>
+      <c r="R10" s="406"/>
+      <c r="S10" s="406"/>
+      <c r="T10" s="406"/>
+      <c r="U10" s="406"/>
       <c r="V10" s="248"/>
       <c r="W10" s="234"/>
       <c r="X10" s="234"/>
-      <c r="Y10" s="384"/>
-      <c r="Z10" s="384"/>
-      <c r="AA10" s="384"/>
-      <c r="AB10" s="385"/>
+      <c r="Y10" s="382"/>
+      <c r="Z10" s="382"/>
+      <c r="AA10" s="382"/>
+      <c r="AB10" s="383"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="114" t="s">
@@ -10773,20 +10924,20 @@
       <c r="N11" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O11" s="390"/>
-      <c r="P11" s="391"/>
-      <c r="Q11" s="391"/>
-      <c r="R11" s="391"/>
-      <c r="S11" s="391"/>
-      <c r="T11" s="391"/>
-      <c r="U11" s="391"/>
+      <c r="O11" s="407"/>
+      <c r="P11" s="408"/>
+      <c r="Q11" s="408"/>
+      <c r="R11" s="408"/>
+      <c r="S11" s="408"/>
+      <c r="T11" s="408"/>
+      <c r="U11" s="408"/>
       <c r="V11" s="247"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="384"/>
-      <c r="Z11" s="384"/>
-      <c r="AA11" s="384"/>
-      <c r="AB11" s="385"/>
+      <c r="Y11" s="382"/>
+      <c r="Z11" s="382"/>
+      <c r="AA11" s="382"/>
+      <c r="AB11" s="383"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B12" s="114" t="s">
@@ -10839,20 +10990,20 @@
       <c r="N12" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O12" s="386"/>
-      <c r="P12" s="387"/>
-      <c r="Q12" s="387"/>
-      <c r="R12" s="387"/>
-      <c r="S12" s="387"/>
-      <c r="T12" s="387"/>
-      <c r="U12" s="387"/>
+      <c r="O12" s="389"/>
+      <c r="P12" s="390"/>
+      <c r="Q12" s="390"/>
+      <c r="R12" s="390"/>
+      <c r="S12" s="390"/>
+      <c r="T12" s="390"/>
+      <c r="U12" s="390"/>
       <c r="V12" s="247"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="384"/>
-      <c r="Z12" s="384"/>
-      <c r="AA12" s="384"/>
-      <c r="AB12" s="385"/>
+      <c r="Y12" s="382"/>
+      <c r="Z12" s="382"/>
+      <c r="AA12" s="382"/>
+      <c r="AB12" s="383"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B13" s="114" t="s">
@@ -10905,20 +11056,20 @@
       <c r="N13" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O13" s="386"/>
-      <c r="P13" s="387"/>
-      <c r="Q13" s="387"/>
-      <c r="R13" s="387"/>
-      <c r="S13" s="387"/>
-      <c r="T13" s="387"/>
-      <c r="U13" s="387"/>
+      <c r="O13" s="389"/>
+      <c r="P13" s="390"/>
+      <c r="Q13" s="390"/>
+      <c r="R13" s="390"/>
+      <c r="S13" s="390"/>
+      <c r="T13" s="390"/>
+      <c r="U13" s="390"/>
       <c r="V13" s="247"/>
       <c r="W13" s="234"/>
       <c r="X13" s="234"/>
-      <c r="Y13" s="384"/>
-      <c r="Z13" s="384"/>
-      <c r="AA13" s="384"/>
-      <c r="AB13" s="385"/>
+      <c r="Y13" s="382"/>
+      <c r="Z13" s="382"/>
+      <c r="AA13" s="382"/>
+      <c r="AB13" s="383"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B14" s="114" t="s">
@@ -10960,22 +11111,22 @@
       <c r="N14" s="259" t="s">
         <v>287</v>
       </c>
-      <c r="O14" s="386" t="s">
+      <c r="O14" s="389" t="s">
         <v>373</v>
       </c>
-      <c r="P14" s="387"/>
-      <c r="Q14" s="387"/>
-      <c r="R14" s="387"/>
-      <c r="S14" s="387"/>
-      <c r="T14" s="387"/>
-      <c r="U14" s="387"/>
+      <c r="P14" s="390"/>
+      <c r="Q14" s="390"/>
+      <c r="R14" s="390"/>
+      <c r="S14" s="390"/>
+      <c r="T14" s="390"/>
+      <c r="U14" s="390"/>
       <c r="V14" s="247"/>
       <c r="W14" s="115"/>
       <c r="X14" s="115"/>
-      <c r="Y14" s="384"/>
-      <c r="Z14" s="384"/>
-      <c r="AA14" s="384"/>
-      <c r="AB14" s="385"/>
+      <c r="Y14" s="382"/>
+      <c r="Z14" s="382"/>
+      <c r="AA14" s="382"/>
+      <c r="AB14" s="383"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B15" s="114" t="s">
@@ -11028,20 +11179,20 @@
       <c r="N15" s="223" t="s">
         <v>287</v>
       </c>
-      <c r="O15" s="386"/>
-      <c r="P15" s="387"/>
-      <c r="Q15" s="387"/>
-      <c r="R15" s="387"/>
-      <c r="S15" s="387"/>
-      <c r="T15" s="387"/>
-      <c r="U15" s="387"/>
+      <c r="O15" s="389"/>
+      <c r="P15" s="390"/>
+      <c r="Q15" s="390"/>
+      <c r="R15" s="390"/>
+      <c r="S15" s="390"/>
+      <c r="T15" s="390"/>
+      <c r="U15" s="390"/>
       <c r="V15" s="250"/>
       <c r="W15" s="58"/>
       <c r="X15" s="58"/>
-      <c r="Y15" s="382"/>
-      <c r="Z15" s="382"/>
-      <c r="AA15" s="382"/>
-      <c r="AB15" s="383"/>
+      <c r="Y15" s="380"/>
+      <c r="Z15" s="380"/>
+      <c r="AA15" s="380"/>
+      <c r="AB15" s="381"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B16" s="113" t="s">
@@ -11084,15 +11235,15 @@
       <c r="N16" s="225" t="s">
         <v>287</v>
       </c>
-      <c r="O16" s="386" t="s">
+      <c r="O16" s="389" t="s">
         <v>374</v>
       </c>
-      <c r="P16" s="387"/>
-      <c r="Q16" s="387"/>
-      <c r="R16" s="387"/>
-      <c r="S16" s="387"/>
-      <c r="T16" s="387"/>
-      <c r="U16" s="387"/>
+      <c r="P16" s="390"/>
+      <c r="Q16" s="390"/>
+      <c r="R16" s="390"/>
+      <c r="S16" s="390"/>
+      <c r="T16" s="390"/>
+      <c r="U16" s="390"/>
       <c r="V16" s="246" t="s">
         <v>361</v>
       </c>
@@ -11117,13 +11268,13 @@
       <c r="L17" s="219"/>
       <c r="M17" s="219"/>
       <c r="N17" s="219"/>
-      <c r="O17" s="400"/>
-      <c r="P17" s="384"/>
-      <c r="Q17" s="384"/>
-      <c r="R17" s="384"/>
-      <c r="S17" s="384"/>
-      <c r="T17" s="384"/>
-      <c r="U17" s="384"/>
+      <c r="O17" s="384"/>
+      <c r="P17" s="382"/>
+      <c r="Q17" s="382"/>
+      <c r="R17" s="382"/>
+      <c r="S17" s="382"/>
+      <c r="T17" s="382"/>
+      <c r="U17" s="382"/>
       <c r="V17" s="247"/>
       <c r="W17" s="251" t="s">
         <v>364</v>
@@ -11175,15 +11326,15 @@
         <f>'Corrected energy balance step 2'!BN90</f>
         <v>0</v>
       </c>
-      <c r="O18" s="407" t="s">
+      <c r="O18" s="387" t="s">
         <v>312</v>
       </c>
-      <c r="P18" s="408"/>
-      <c r="Q18" s="408"/>
-      <c r="R18" s="408"/>
-      <c r="S18" s="408"/>
-      <c r="T18" s="408"/>
-      <c r="U18" s="408"/>
+      <c r="P18" s="388"/>
+      <c r="Q18" s="388"/>
+      <c r="R18" s="388"/>
+      <c r="S18" s="388"/>
+      <c r="T18" s="388"/>
+      <c r="U18" s="388"/>
       <c r="V18" s="247"/>
       <c r="AB18" s="235"/>
     </row>
@@ -11201,13 +11352,13 @@
       <c r="L19" s="221"/>
       <c r="M19" s="221"/>
       <c r="N19" s="221"/>
-      <c r="O19" s="405"/>
-      <c r="P19" s="406"/>
-      <c r="Q19" s="406"/>
-      <c r="R19" s="406"/>
-      <c r="S19" s="406"/>
-      <c r="T19" s="406"/>
-      <c r="U19" s="406"/>
+      <c r="O19" s="385"/>
+      <c r="P19" s="386"/>
+      <c r="Q19" s="386"/>
+      <c r="R19" s="386"/>
+      <c r="S19" s="386"/>
+      <c r="T19" s="386"/>
+      <c r="U19" s="386"/>
       <c r="V19" s="247"/>
       <c r="W19" s="201" t="s">
         <v>365</v>
@@ -11235,13 +11386,13 @@
       <c r="L20" s="263"/>
       <c r="M20" s="263"/>
       <c r="N20" s="263"/>
-      <c r="O20" s="400"/>
-      <c r="P20" s="384"/>
-      <c r="Q20" s="384"/>
-      <c r="R20" s="384"/>
-      <c r="S20" s="384"/>
-      <c r="T20" s="384"/>
-      <c r="U20" s="384"/>
+      <c r="O20" s="384"/>
+      <c r="P20" s="382"/>
+      <c r="Q20" s="382"/>
+      <c r="R20" s="382"/>
+      <c r="S20" s="382"/>
+      <c r="T20" s="382"/>
+      <c r="U20" s="382"/>
       <c r="V20" s="247"/>
       <c r="W20" s="201" t="s">
         <v>366</v>
@@ -11306,13 +11457,13 @@
       <c r="N21" s="227" t="s">
         <v>287</v>
       </c>
-      <c r="O21" s="405"/>
-      <c r="P21" s="406"/>
-      <c r="Q21" s="406"/>
-      <c r="R21" s="406"/>
-      <c r="S21" s="406"/>
-      <c r="T21" s="406"/>
-      <c r="U21" s="406"/>
+      <c r="O21" s="385"/>
+      <c r="P21" s="386"/>
+      <c r="Q21" s="386"/>
+      <c r="R21" s="386"/>
+      <c r="S21" s="386"/>
+      <c r="T21" s="386"/>
+      <c r="U21" s="386"/>
       <c r="V21" s="247"/>
       <c r="W21" s="234"/>
       <c r="X21" s="234"/>
@@ -11362,13 +11513,13 @@
         <f>N18</f>
         <v>0</v>
       </c>
-      <c r="O22" s="405"/>
-      <c r="P22" s="406"/>
-      <c r="Q22" s="406"/>
-      <c r="R22" s="406"/>
-      <c r="S22" s="406"/>
-      <c r="T22" s="406"/>
-      <c r="U22" s="406"/>
+      <c r="O22" s="385"/>
+      <c r="P22" s="386"/>
+      <c r="Q22" s="386"/>
+      <c r="R22" s="386"/>
+      <c r="S22" s="386"/>
+      <c r="T22" s="386"/>
+      <c r="U22" s="386"/>
       <c r="V22" s="247"/>
       <c r="W22" s="234"/>
       <c r="X22" s="234"/>
@@ -11404,13 +11555,13 @@
       <c r="L23" s="266"/>
       <c r="M23" s="266"/>
       <c r="N23" s="266"/>
-      <c r="O23" s="403"/>
-      <c r="P23" s="404"/>
-      <c r="Q23" s="404"/>
-      <c r="R23" s="404"/>
-      <c r="S23" s="404"/>
-      <c r="T23" s="404"/>
-      <c r="U23" s="404"/>
+      <c r="O23" s="378"/>
+      <c r="P23" s="379"/>
+      <c r="Q23" s="379"/>
+      <c r="R23" s="379"/>
+      <c r="S23" s="379"/>
+      <c r="T23" s="379"/>
+      <c r="U23" s="379"/>
       <c r="V23" s="249"/>
       <c r="W23" s="237"/>
       <c r="X23" s="237"/>
@@ -11436,14 +11587,31 @@
       <c r="V24" s="234"/>
       <c r="W24" s="115"/>
       <c r="X24" s="115"/>
-      <c r="Y24" s="384"/>
-      <c r="Z24" s="384"/>
-      <c r="AA24" s="384"/>
-      <c r="AB24" s="384"/>
+      <c r="Y24" s="382"/>
+      <c r="Z24" s="382"/>
+      <c r="AA24" s="382"/>
+      <c r="AB24" s="382"/>
       <c r="AC24" s="234"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Y7:AB7"/>
+    <mergeCell ref="Y8:AB8"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="Y14:AB14"/>
+    <mergeCell ref="O13:U13"/>
+    <mergeCell ref="O14:U14"/>
+    <mergeCell ref="Y10:AB10"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="Y12:AB12"/>
+    <mergeCell ref="O10:U10"/>
+    <mergeCell ref="O11:U11"/>
+    <mergeCell ref="O12:U12"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="O8:T8"/>
+    <mergeCell ref="O9:T9"/>
     <mergeCell ref="O23:U23"/>
     <mergeCell ref="Y15:AB15"/>
     <mergeCell ref="Y24:AB24"/>
@@ -11456,23 +11624,6 @@
     <mergeCell ref="O15:U15"/>
     <mergeCell ref="O16:U16"/>
     <mergeCell ref="O17:U17"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="O8:T8"/>
-    <mergeCell ref="O9:T9"/>
-    <mergeCell ref="Y7:AB7"/>
-    <mergeCell ref="Y8:AB8"/>
-    <mergeCell ref="Y9:AB9"/>
-    <mergeCell ref="Y14:AB14"/>
-    <mergeCell ref="O13:U13"/>
-    <mergeCell ref="O14:U14"/>
-    <mergeCell ref="Y10:AB10"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="Y12:AB12"/>
-    <mergeCell ref="O10:U10"/>
-    <mergeCell ref="O11:U11"/>
-    <mergeCell ref="O12:U12"/>
   </mergeCells>
   <conditionalFormatting sqref="X19:X20">
     <cfRule type="duplicateValues" dxfId="2" priority="5"/>
@@ -11489,8 +11640,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet12">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -11543,8 +11694,8 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet13">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
@@ -11612,8 +11763,8 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet14" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet14">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -11645,18 +11796,18 @@
       <c r="A3" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="155" t="e">
+      <c r="B3" s="155">
         <f>'Application Shares'!E22</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="96" t="s">
         <v>226</v>
       </c>
-      <c r="B4" s="155" t="e">
+      <c r="B4" s="155">
         <f>'Application Shares'!E21</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11666,8 +11817,8 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet15">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -11727,8 +11878,8 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet16" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sheet16">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -11784,8 +11935,8 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet17" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet17">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
@@ -11865,8 +12016,8 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet18" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet18">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:L17"/>
@@ -11970,8 +12121,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:D29"/>
@@ -12213,8 +12364,8 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet19" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr codeName="Sheet19">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -12276,8 +12427,8 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
@@ -12339,8 +12490,8 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G8"/>
@@ -12425,8 +12576,8 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:F5"/>
@@ -12490,8 +12641,8 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet20" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr codeName="Sheet20">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -12553,8 +12704,8 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -12607,8 +12758,8 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -12658,8 +12809,8 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -12714,8 +12865,8 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
@@ -12793,8 +12944,8 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -12849,8 +13000,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet4">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:B21"/>
@@ -12949,8 +13100,8 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
@@ -12992,8 +13143,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet3">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:C30"/>
@@ -13234,8 +13385,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:BQ12"/>
@@ -13605,8 +13756,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:I111"/>
@@ -14303,13 +14454,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:Y75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
@@ -16005,7 +16156,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number Range" error="This cell can only contain a number between 0% and 100%" sqref="E24 E28:E29 E32:E34 E38:E40 E58:E59 E62:E63 E44:E46 E48:E52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number Range" error="This cell can only contain a number between 0% and 100%" sqref="E24 E28:E29 E32:E34 E38:E40 E58:E59 E62:E63 E44:E46 E48:E52" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -16020,7 +16171,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="9222" r:id="rId3" name="import_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!import_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!import_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -16038,12 +16189,11 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="9223" r:id="rId4" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!export_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!export_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -16061,12 +16211,11 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="9224" r:id="rId5" name="select_dashboard">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!select_dashboard_values">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!select_dashboard_values">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -16084,18 +16233,16 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:BS101"/>
@@ -22942,14 +23089,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23148,9 +23295,9 @@
         <f>'Fuel Aggregation'!J11</f>
         <v>0</v>
       </c>
-      <c r="E21" s="121" t="e">
-        <f>D21/SUM($D$21:$D$22)</f>
-        <v>#DIV/0!</v>
+      <c r="E21" s="121">
+        <f>IF(SUM(D21:D22)=0,0, D21/SUM($D$21:$D$22))</f>
+        <v>0</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -23163,9 +23310,9 @@
         <f>'Fuel Aggregation'!J12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="121" t="e">
-        <f>D22/SUM($D$21:$D$22)</f>
-        <v>#DIV/0!</v>
+      <c r="E22" s="121">
+        <f>IF(SUM(D21:D22)=0,1,D22/SUM($D$21:$D$22))</f>
+        <v>1</v>
       </c>
       <c r="F22" s="8"/>
     </row>

</xml_diff>